<commit_message>
Fix bug open browser
</commit_message>
<xml_diff>
--- a/src/test/java/dataEngine/DataEngine.xlsx
+++ b/src/test/java/dataEngine/DataEngine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Automation\working\SendID\senid\src\test\java\dataEngine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54FA3780-9A34-420E-A3ED-630A5E1FF8D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01FBC2AC-C9C5-488F-AE83-BFB22CB5B787}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="1650" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{81D78742-11F9-4B4A-A9D3-448BFA7463DC}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="88">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -306,13 +306,10 @@
     <t>TS_015</t>
   </si>
   <si>
+    <t>FAIL</t>
+  </si>
+  <si>
     <t>chrome</t>
-  </si>
-  <si>
-    <t>FAIL</t>
-  </si>
-  <si>
-    <t>edge</t>
   </si>
 </sst>
 </file>
@@ -749,7 +746,7 @@
         <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.45">
@@ -763,7 +760,7 @@
         <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -777,7 +774,7 @@
   <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -829,10 +826,10 @@
         <v>16</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.45">
@@ -1142,10 +1139,10 @@
         <v>16</v>
       </c>
       <c r="G17" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="H17" t="s">
         <v>86</v>
-      </c>
-      <c r="H17" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
Update test case dang ky
</commit_message>
<xml_diff>
--- a/src/test/java/dataEngine/DataEngine.xlsx
+++ b/src/test/java/dataEngine/DataEngine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Automation\working\SendID\senid\src\test\java\dataEngine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3EDEF69-D3AB-4B79-AB52-E102DDD5CAF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69FDBC39-5EF4-4FB7-8C31-B2F92F73DE2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="1650" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{81D78742-11F9-4B4A-A9D3-448BFA7463DC}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="156">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -273,136 +273,244 @@
     <t>Hover mouse to Login button</t>
   </si>
   <si>
+    <t>chrome</t>
+  </si>
+  <si>
+    <t>123456Ab</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Click on Dang Nhap button</t>
+  </si>
+  <si>
+    <t>login_Btn1</t>
+  </si>
+  <si>
+    <t>login_Btn2</t>
+  </si>
+  <si>
+    <t>TS_018</t>
+  </si>
+  <si>
+    <t>TS_019</t>
+  </si>
+  <si>
+    <t>TS_020</t>
+  </si>
+  <si>
+    <t>TS_021</t>
+  </si>
+  <si>
+    <t>TS_022</t>
+  </si>
+  <si>
+    <t>TS_023</t>
+  </si>
+  <si>
+    <t>TS_024</t>
+  </si>
+  <si>
+    <t>TS_025</t>
+  </si>
+  <si>
+    <t>TS_026</t>
+  </si>
+  <si>
+    <t>TS_027</t>
+  </si>
+  <si>
+    <t>TS_028</t>
+  </si>
+  <si>
+    <t>TS_003</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>search_Tbx</t>
+  </si>
+  <si>
+    <t>TS_013</t>
+  </si>
+  <si>
+    <t>TS_014</t>
+  </si>
+  <si>
+    <t>TS_015</t>
+  </si>
+  <si>
+    <t>TS_016</t>
+  </si>
+  <si>
+    <t>TS_017</t>
+  </si>
+  <si>
+    <t>TS_011</t>
+  </si>
+  <si>
+    <t>TS_029</t>
+  </si>
+  <si>
+    <t>Waiting for search bar</t>
+  </si>
+  <si>
+    <t>TS_012</t>
+  </si>
+  <si>
+    <t>Press Enter search bar</t>
+  </si>
+  <si>
+    <t>Hover mouse to search bar</t>
+  </si>
+  <si>
+    <t>TS_030</t>
+  </si>
+  <si>
+    <t>Input the cource in search bar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Input the Username </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Input the Password </t>
+  </si>
+  <si>
+    <t>TS_031</t>
+  </si>
+  <si>
+    <t>TS_004</t>
+  </si>
+  <si>
+    <t>TS_005</t>
+  </si>
+  <si>
+    <t>TS_006</t>
+  </si>
+  <si>
+    <t>TS_007</t>
+  </si>
+  <si>
+    <t>searchSuggestion_Tbx</t>
+  </si>
+  <si>
+    <t>Automation Testing</t>
+  </si>
+  <si>
+    <t>Click on cource "Automation Testing"</t>
+  </si>
+  <si>
+    <t>courceResult</t>
+  </si>
+  <si>
+    <t>Click on Dang Ky button</t>
+  </si>
+  <si>
+    <t>registerCource_Btn</t>
+  </si>
+  <si>
+    <t>Click on "Vao hoc ngay" button</t>
+  </si>
+  <si>
+    <t>vaoHocNgay_Btn</t>
+  </si>
+  <si>
+    <t>chonKhungGioHoc_Btn</t>
+  </si>
+  <si>
+    <t>TS_032</t>
+  </si>
+  <si>
+    <t>TS_033</t>
+  </si>
+  <si>
+    <t>TS_034</t>
+  </si>
+  <si>
+    <t>TS_035</t>
+  </si>
+  <si>
+    <t>TS_036</t>
+  </si>
+  <si>
+    <t>scrollToElement</t>
+  </si>
+  <si>
+    <t>thongstudent010@yopmail.com</t>
+  </si>
+  <si>
+    <t>ngayHoc_list</t>
+  </si>
+  <si>
+    <t>selectValueFromDropDown</t>
+  </si>
+  <si>
     <t>FAIL</t>
   </si>
   <si>
-    <t>chrome</t>
-  </si>
-  <si>
-    <t>123456Ab</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Click on Dang Nhap button</t>
-  </si>
-  <si>
-    <t>login_Btn1</t>
-  </si>
-  <si>
-    <t>login_Btn2</t>
-  </si>
-  <si>
-    <t>TS_018</t>
-  </si>
-  <si>
-    <t>TS_019</t>
-  </si>
-  <si>
-    <t>TS_020</t>
-  </si>
-  <si>
-    <t>TS_021</t>
-  </si>
-  <si>
-    <t>TS_022</t>
-  </si>
-  <si>
-    <t>TS_023</t>
-  </si>
-  <si>
-    <t>TS_024</t>
-  </si>
-  <si>
-    <t>TS_025</t>
-  </si>
-  <si>
-    <t>TS_026</t>
-  </si>
-  <si>
-    <t>TS_027</t>
-  </si>
-  <si>
-    <t>TS_028</t>
-  </si>
-  <si>
-    <t>TS_003</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>search_Tbx</t>
-  </si>
-  <si>
-    <t>TS_013</t>
-  </si>
-  <si>
-    <t>TS_014</t>
-  </si>
-  <si>
-    <t>TS_015</t>
-  </si>
-  <si>
-    <t>TS_016</t>
-  </si>
-  <si>
-    <t>TS_017</t>
-  </si>
-  <si>
-    <t>thongstudent002@yopmail.com</t>
-  </si>
-  <si>
-    <t>TS_011</t>
-  </si>
-  <si>
-    <t>TS_029</t>
-  </si>
-  <si>
-    <t>Waiting for search bar</t>
-  </si>
-  <si>
-    <t>TS_012</t>
-  </si>
-  <si>
-    <t>Press Enter search bar</t>
-  </si>
-  <si>
-    <t>pressEnter</t>
-  </si>
-  <si>
-    <t>Hover mouse to search bar</t>
-  </si>
-  <si>
-    <t>TS_030</t>
-  </si>
-  <si>
-    <t>Input the cource in search bar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Input the Username </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Input the Password </t>
-  </si>
-  <si>
-    <t>Automation testing</t>
-  </si>
-  <si>
-    <t>TS_031</t>
-  </si>
-  <si>
-    <t>TS_032</t>
-  </si>
-  <si>
-    <t>TS_033</t>
-  </si>
-  <si>
-    <t>TS_034</t>
-  </si>
-  <si>
-    <t>Wait for 5 s</t>
+    <t>Waiting for Chon Khung Gio Hoc</t>
+  </si>
+  <si>
+    <t>Click on Chon Khung Gio Hoc</t>
+  </si>
+  <si>
+    <t>luuThayDoi_Btn</t>
+  </si>
+  <si>
+    <t>Cick button Luu Thay Doi</t>
+  </si>
+  <si>
+    <t>Cick button Vao Hoc Ngay</t>
+  </si>
+  <si>
+    <t>selectIndexFromDropDown</t>
+  </si>
+  <si>
+    <t>lichCoDinh_Radio</t>
+  </si>
+  <si>
+    <t>Chon lich co dinh</t>
+  </si>
+  <si>
+    <t>TS_037</t>
+  </si>
+  <si>
+    <t>TS_038</t>
+  </si>
+  <si>
+    <t>TS_039</t>
+  </si>
+  <si>
+    <t>TS_040</t>
+  </si>
+  <si>
+    <t>Chon lich tu chon</t>
+  </si>
+  <si>
+    <t>lichTuChon_Radio</t>
+  </si>
+  <si>
+    <t>timesheet</t>
+  </si>
+  <si>
+    <t>Click on Time Sheet</t>
+  </si>
+  <si>
+    <t>Chon ngay hoc</t>
+  </si>
+  <si>
+    <t>sendKey</t>
+  </si>
+  <si>
+    <t>ENTER</t>
+  </si>
+  <si>
+    <t>ngayHoc_option</t>
+  </si>
+  <si>
+    <t>https://senid.banvien.com.vn/</t>
   </si>
   <si>
     <t>PASS</t>
@@ -787,8 +895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4F1EDE2-3E0B-4E49-8C42-F221926AB428}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="R20" sqref="R20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -821,7 +929,7 @@
         <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>75</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.45">
@@ -832,10 +940,7 @@
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>78</v>
-      </c>
-      <c r="D3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -846,10 +951,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A696EC6A-F50E-4D7B-ABB3-CDE9DA0E200A}">
-  <dimension ref="A1:N38"/>
+  <dimension ref="A1:K47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P17" sqref="P17"/>
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -861,7 +966,7 @@
     <col min="7" max="7" customWidth="true" width="12.53125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -889,11 +994,8 @@
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -909,19 +1011,16 @@
         <v>16</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H2" t="s">
-        <v>119</v>
+        <v>155</v>
       </c>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -936,23 +1035,22 @@
       <c r="F3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="4"/>
+      <c r="G3" s="2" t="s">
+        <v>154</v>
+      </c>
       <c r="H3" t="s">
-        <v>119</v>
+        <v>155</v>
       </c>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>73</v>
@@ -961,30 +1059,27 @@
         <v>21</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>40</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H4" t="s">
-        <v>119</v>
+        <v>155</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>35</v>
+        <v>111</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>74</v>
@@ -993,61 +1088,55 @@
         <v>21</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>34</v>
       </c>
       <c r="G5" s="5"/>
       <c r="H5" t="s">
-        <v>119</v>
+        <v>155</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>38</v>
+        <v>112</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>62</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>31</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" t="s">
-        <v>119</v>
+        <v>155</v>
       </c>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>42</v>
+        <v>113</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>62</v>
@@ -1059,27 +1148,24 @@
         <v>23</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>101</v>
+        <v>130</v>
       </c>
       <c r="H7" t="s">
-        <v>119</v>
+        <v>155</v>
       </c>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>102</v>
+        <v>114</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>21</v>
@@ -1091,24 +1177,21 @@
         <v>23</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H8" t="s">
-        <v>119</v>
+        <v>155</v>
       </c>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="3"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A9" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>105</v>
+        <v>35</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>73</v>
@@ -1117,7 +1200,7 @@
         <v>21</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>40</v>
@@ -1126,21 +1209,18 @@
         <v>41</v>
       </c>
       <c r="H9" t="s">
-        <v>119</v>
+        <v>155</v>
       </c>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
-      <c r="N9" s="3"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A10" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>96</v>
+        <v>38</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>74</v>
@@ -1149,28 +1229,25 @@
         <v>21</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>34</v>
       </c>
       <c r="G10" s="5"/>
       <c r="H10" t="s">
-        <v>119</v>
+        <v>155</v>
       </c>
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
-      <c r="N10" s="3"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.45">
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A11" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>97</v>
+        <v>42</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>29</v>
@@ -1179,37 +1256,34 @@
         <v>21</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>31</v>
       </c>
       <c r="G11" s="4"/>
       <c r="H11" t="s">
-        <v>119</v>
+        <v>155</v>
       </c>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
-      <c r="M11" s="3"/>
-      <c r="N11" s="3"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.45">
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A12" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>37</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>40</v>
@@ -1218,679 +1292,865 @@
         <v>41</v>
       </c>
       <c r="H12" t="s">
-        <v>119</v>
+        <v>155</v>
       </c>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
-      <c r="N12" s="3"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.45">
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A13" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>37</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>34</v>
       </c>
       <c r="G13" s="5"/>
       <c r="H13" t="s">
-        <v>119</v>
+        <v>155</v>
       </c>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
-      <c r="M13" s="3"/>
-      <c r="N13" s="3"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.45">
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A14" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>62</v>
+        <v>37</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>23</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="H14" t="s">
-        <v>119</v>
+        <v>155</v>
       </c>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
-      <c r="M14" s="3"/>
-      <c r="N14" s="3"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.45">
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A15" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E15" s="3"/>
+      <c r="E15" s="3" t="s">
+        <v>115</v>
+      </c>
       <c r="F15" s="3" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="G15" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="H15" s="3"/>
+      <c r="H15" t="s">
+        <v>155</v>
+      </c>
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
-      <c r="L15" s="3"/>
-      <c r="M15" s="3"/>
-      <c r="N15" s="3"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.45">
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A16" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>82</v>
+        <v>97</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>37</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="G16" s="5"/>
-      <c r="H16" s="3"/>
+        <v>151</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="H16" t="s">
+        <v>155</v>
+      </c>
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
-      <c r="M16" s="3"/>
-      <c r="N16" s="3"/>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.45">
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A17" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>83</v>
+        <v>98</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
+        <v>117</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>118</v>
+      </c>
       <c r="F17" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
+        <v>31</v>
+      </c>
+      <c r="G17" s="4"/>
+      <c r="H17" t="s">
+        <v>155</v>
+      </c>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
-      <c r="M17" s="3"/>
-      <c r="N17" s="3"/>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.45">
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A18" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>84</v>
+        <v>99</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
+        <v>119</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>120</v>
+      </c>
       <c r="F18" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="H18" s="3"/>
+        <v>31</v>
+      </c>
+      <c r="G18" s="4"/>
+      <c r="H18" t="s">
+        <v>155</v>
+      </c>
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
-      <c r="M18" s="3"/>
-      <c r="N18" s="3"/>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.45">
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A19" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
+        <v>121</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>122</v>
+      </c>
       <c r="F19" s="3" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="G19" s="4"/>
-      <c r="H19" s="3"/>
+      <c r="H19" t="s">
+        <v>155</v>
+      </c>
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
-      <c r="L19" s="3"/>
-      <c r="M19" s="3"/>
-      <c r="N19" s="3"/>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.45">
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A20" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>20</v>
+        <v>134</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>62</v>
+        <v>37</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>22</v>
+        <v>123</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="H20" s="3"/>
+        <v>40</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="H20" t="s">
+        <v>133</v>
+      </c>
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
-      <c r="L20" s="3"/>
-      <c r="M20" s="3"/>
-      <c r="N20" s="3"/>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.45">
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A21" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>26</v>
+        <v>135</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>27</v>
+        <v>123</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>70</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="G21" s="5"/>
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
-      <c r="L21" s="3"/>
-      <c r="M21" s="3"/>
-      <c r="N21" s="3"/>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.45">
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A22" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>73</v>
+        <v>146</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>30</v>
+        <v>147</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="G22" s="5" t="s">
-        <v>41</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="G22" s="5"/>
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
-      <c r="L22" s="3"/>
-      <c r="M22" s="3"/>
-      <c r="N22" s="3"/>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.45">
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A23" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>74</v>
+        <v>141</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>30</v>
+        <v>140</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G23" s="5"/>
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
-      <c r="L23" s="3"/>
-      <c r="M23" s="3"/>
-      <c r="N23" s="3"/>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.45">
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A24" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>29</v>
+        <v>149</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>30</v>
+        <v>148</v>
       </c>
       <c r="F24" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="G24" s="4"/>
+      <c r="G24" s="5"/>
       <c r="H24" s="3"/>
       <c r="I24" s="3"/>
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
-      <c r="L24" s="3"/>
-      <c r="M24" s="3"/>
-      <c r="N24" s="3"/>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.45">
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A25" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>72</v>
+        <v>150</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>37</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>59</v>
+        <v>153</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="G25" s="5" t="s">
-        <v>41</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="G25" s="5"/>
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
-      <c r="L25" s="3"/>
-      <c r="M25" s="3"/>
-      <c r="N25" s="3"/>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.45">
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A26" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>32</v>
+        <v>137</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>37</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>33</v>
+        <v>136</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="G26" s="4"/>
+        <v>31</v>
+      </c>
+      <c r="G26" s="5"/>
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
       <c r="J26" s="3"/>
       <c r="K26" s="3"/>
-      <c r="L26" s="3"/>
-      <c r="M26" s="3"/>
-      <c r="N26" s="3"/>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.45">
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A27" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>36</v>
+        <v>138</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>37</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>33</v>
+        <v>122</v>
       </c>
       <c r="F27" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="G27" s="4"/>
+      <c r="G27" s="5"/>
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
-      <c r="L27" s="3"/>
-      <c r="M27" s="3"/>
-      <c r="N27" s="3"/>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.45">
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A28" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>109</v>
+        <v>88</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>39</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
       <c r="F28" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="G28" s="5" t="s">
-        <v>41</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="G28" s="3"/>
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
       <c r="J28" s="3"/>
       <c r="K28" s="3"/>
-      <c r="L28" s="3"/>
-      <c r="M28" s="3"/>
-      <c r="N28" s="3"/>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.45">
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A29" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>114</v>
+        <v>89</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>39</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
       <c r="F29" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="G29" s="4"/>
+        <v>16</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>75</v>
+      </c>
       <c r="H29" s="3"/>
       <c r="I29" s="3"/>
       <c r="J29" s="3"/>
       <c r="K29" s="3"/>
-      <c r="L29" s="3"/>
-      <c r="M29" s="3"/>
-      <c r="N29" s="3"/>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.45">
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A30" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>115</v>
+        <v>90</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>39</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
       <c r="F30" s="3" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="G30" s="4"/>
       <c r="H30" s="3"/>
       <c r="I30" s="3"/>
       <c r="J30" s="3"/>
       <c r="K30" s="3"/>
-      <c r="L30" s="3"/>
-      <c r="M30" s="3"/>
-      <c r="N30" s="3"/>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.45">
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A31" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>116</v>
+        <v>91</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>67</v>
+        <v>20</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>63</v>
+        <v>22</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="G31" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G31" s="4" t="s">
         <v>69</v>
       </c>
       <c r="H31" s="3"/>
       <c r="I31" s="3"/>
       <c r="J31" s="3"/>
       <c r="K31" s="3"/>
-      <c r="L31" s="3"/>
-      <c r="M31" s="3"/>
-      <c r="N31" s="3"/>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.45">
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A32" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
+        <v>26</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="F32" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="G32" s="3"/>
+        <v>23</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>70</v>
+      </c>
       <c r="H32" s="3"/>
       <c r="I32" s="3"/>
       <c r="J32" s="3"/>
       <c r="K32" s="3"/>
-      <c r="L32" s="3"/>
-      <c r="M32" s="3"/>
-      <c r="N32" s="3"/>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A33" s="3"/>
-      <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="3"/>
-      <c r="G33" s="3"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A33" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>41</v>
+      </c>
       <c r="H33" s="3"/>
       <c r="I33" s="3"/>
       <c r="J33" s="3"/>
       <c r="K33" s="3"/>
-      <c r="L33" s="3"/>
-      <c r="M33" s="3"/>
-      <c r="N33" s="3"/>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A34" s="3"/>
-      <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="3"/>
-      <c r="G34" s="3"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A34" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G34" s="5"/>
       <c r="H34" s="3"/>
       <c r="I34" s="3"/>
       <c r="J34" s="3"/>
       <c r="K34" s="3"/>
-      <c r="L34" s="3"/>
-      <c r="M34" s="3"/>
-      <c r="N34" s="3"/>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A35" s="3"/>
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="3"/>
-      <c r="G35" s="3"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A35" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G35" s="4"/>
       <c r="H35" s="3"/>
       <c r="I35" s="3"/>
       <c r="J35" s="3"/>
       <c r="K35" s="3"/>
-      <c r="L35" s="3"/>
-      <c r="M35" s="3"/>
-      <c r="N35" s="3"/>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A36" s="3"/>
-      <c r="B36" s="3"/>
-      <c r="C36" s="3"/>
-      <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="3"/>
-      <c r="G36" s="3"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A36" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="G36" s="5" t="s">
+        <v>41</v>
+      </c>
       <c r="H36" s="3"/>
       <c r="I36" s="3"/>
       <c r="J36" s="3"/>
       <c r="K36" s="3"/>
-      <c r="L36" s="3"/>
-      <c r="M36" s="3"/>
-      <c r="N36" s="3"/>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A37" s="3"/>
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="3"/>
-      <c r="G37" s="3"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A37" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G37" s="4"/>
       <c r="H37" s="3"/>
       <c r="I37" s="3"/>
       <c r="J37" s="3"/>
       <c r="K37" s="3"/>
-      <c r="L37" s="3"/>
-      <c r="M37" s="3"/>
-      <c r="N37" s="3"/>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A38" s="3"/>
-      <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
-      <c r="G38" s="3"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A38" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G38" s="4"/>
       <c r="H38" s="3"/>
       <c r="I38" s="3"/>
       <c r="J38" s="3"/>
       <c r="K38" s="3"/>
-      <c r="L38" s="3"/>
-      <c r="M38" s="3"/>
-      <c r="N38" s="3"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A39" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G39" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="H39" s="3"/>
+      <c r="I39" s="3"/>
+      <c r="J39" s="3"/>
+      <c r="K39" s="3"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A40" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G40" s="4"/>
+      <c r="H40" s="3"/>
+      <c r="I40" s="3"/>
+      <c r="J40" s="3"/>
+      <c r="K40" s="3"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A41" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G41" s="4"/>
+      <c r="H41" s="3"/>
+      <c r="I41" s="3"/>
+      <c r="J41" s="3"/>
+      <c r="K41" s="3"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A42" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G42" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="H42" s="3"/>
+      <c r="I42" s="3"/>
+      <c r="J42" s="3"/>
+      <c r="K42" s="3"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A43" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G43" s="3"/>
+      <c r="H43" s="3"/>
+      <c r="I43" s="3"/>
+      <c r="J43" s="3"/>
+      <c r="K43" s="3"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A44" s="3"/>
+      <c r="B44" s="3"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3"/>
+      <c r="G44" s="3"/>
+      <c r="H44" s="3"/>
+      <c r="I44" s="3"/>
+      <c r="J44" s="3"/>
+      <c r="K44" s="3"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A45" s="3"/>
+      <c r="B45" s="3"/>
+      <c r="C45" s="3"/>
+      <c r="D45" s="3"/>
+      <c r="E45" s="3"/>
+      <c r="F45" s="3"/>
+      <c r="G45" s="3"/>
+      <c r="H45" s="3"/>
+      <c r="I45" s="3"/>
+      <c r="J45" s="3"/>
+      <c r="K45" s="3"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A46" s="3"/>
+      <c r="B46" s="3"/>
+      <c r="C46" s="3"/>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3"/>
+      <c r="G46" s="3"/>
+      <c r="H46" s="3"/>
+      <c r="I46" s="3"/>
+      <c r="J46" s="3"/>
+      <c r="K46" s="3"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A47" s="3"/>
+      <c r="B47" s="3"/>
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3"/>
+      <c r="F47" s="3"/>
+      <c r="G47" s="3"/>
+      <c r="H47" s="3"/>
+      <c r="I47" s="3"/>
+      <c r="J47" s="3"/>
+      <c r="K47" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D32" xr:uid="{710BACEF-CE5A-4C56-B5C5-5E1AC5E70F66}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D43" xr:uid="{710BACEF-CE5A-4C56-B5C5-5E1AC5E70F66}">
       <formula1>Page_Name</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F1048576" xr:uid="{8405667A-AA8D-489C-B5B3-B6EA9D6474AC}">
@@ -1899,9 +2159,10 @@
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="G7" r:id="rId1" xr:uid="{A037A5DD-8D7E-4EB7-8B48-DAD212B537F3}"/>
+    <hyperlink ref="G3" r:id="rId2" xr:uid="{42283EFE-4D4F-49BA-A138-E02C3F803720}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -1969,10 +2230,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E039E608-272C-4340-A7D2-E2A9089EF229}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2078,30 +2339,86 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E8" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B9" t="s">
+        <v>115</v>
+      </c>
       <c r="E9" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B10" t="s">
+        <v>118</v>
+      </c>
       <c r="E10" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B11" t="s">
+        <v>120</v>
+      </c>
       <c r="E11" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B12" t="s">
+        <v>122</v>
+      </c>
       <c r="E12" t="s">
-        <v>107</v>
+        <v>151</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B13" t="s">
+        <v>123</v>
+      </c>
+      <c r="E13" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B14" t="s">
+        <v>131</v>
+      </c>
+      <c r="E14" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B15" t="s">
+        <v>136</v>
+      </c>
+      <c r="E15" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B16" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B17" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B18" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B19" t="s">
+        <v>153</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update test case GV vao cham bai
</commit_message>
<xml_diff>
--- a/src/test/java/dataEngine/DataEngine.xlsx
+++ b/src/test/java/dataEngine/DataEngine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Automation\working\SendID\senid\src\test\java\dataEngine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{016E16BB-F67F-4B96-8CFD-5B54E74DCEBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A12456B-D093-4CFF-B79C-28886B7609DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="1650" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{81D78742-11F9-4B4A-A9D3-448BFA7463DC}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="217">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -531,10 +531,172 @@
     <t>TS_043</t>
   </si>
   <si>
+    <t>Cource_Page</t>
+  </si>
+  <si>
+    <t>Go To Khoa Hoc Automation Testing</t>
+  </si>
+  <si>
+    <t>tiepTucHoc_Btn</t>
+  </si>
+  <si>
+    <t>Go To Noi Dung Khoa Hoc</t>
+  </si>
+  <si>
+    <t>noiDungKhoaHoc_Tab</t>
+  </si>
+  <si>
+    <t>Go To Chuong 1</t>
+  </si>
+  <si>
+    <t>chuong1_Tab</t>
+  </si>
+  <si>
+    <t>baiCamKet_Tab</t>
+  </si>
+  <si>
+    <t>Accept "Bai Cam Ket"</t>
+  </si>
+  <si>
+    <t>dongYCamKet_Btn</t>
+  </si>
+  <si>
+    <t>baiThucHanh_Tab</t>
+  </si>
+  <si>
+    <t>Do "Bai Thuc Hanh" with text only</t>
+  </si>
+  <si>
+    <t>essay_Txb</t>
+  </si>
+  <si>
+    <t>Ngoi nha than thuong cua chung em</t>
+  </si>
+  <si>
+    <t>Click on "Hoan Thanh" button</t>
+  </si>
+  <si>
+    <t>hoanThanh_Btn</t>
+  </si>
+  <si>
+    <t>FAIL</t>
+  </si>
+  <si>
+    <t>Click on "Bai Thuc Hanh" tab</t>
+  </si>
+  <si>
+    <t>Click on "Bai Cam Ket" tab</t>
+  </si>
+  <si>
+    <t>Wait for "Bai Thuc Hanh" tab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click on "Dang Xuat" button </t>
+  </si>
+  <si>
+    <t>logout_Btn</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>Click on profile icon</t>
+  </si>
+  <si>
+    <t>profile_Ic</t>
+  </si>
+  <si>
+    <t>Wait for essay text box</t>
+  </si>
+  <si>
+    <t>TS_044</t>
+  </si>
+  <si>
+    <t>TS_045</t>
+  </si>
+  <si>
+    <t>TS_046</t>
+  </si>
+  <si>
+    <t>TS_047</t>
+  </si>
+  <si>
+    <t>TS_048</t>
+  </si>
+  <si>
+    <t>TS_049</t>
+  </si>
+  <si>
+    <t>TS_050</t>
+  </si>
+  <si>
+    <t>TS_051</t>
+  </si>
+  <si>
+    <t>TS_052</t>
+  </si>
+  <si>
+    <t>TS_053</t>
+  </si>
+  <si>
+    <t>TS_054</t>
+  </si>
+  <si>
+    <t>TS_055</t>
+  </si>
+  <si>
+    <t>thongteacher001@yopmail.com</t>
+  </si>
+  <si>
+    <t>TS_056</t>
+  </si>
+  <si>
+    <t>TS_057</t>
+  </si>
+  <si>
+    <t>TS_058</t>
+  </si>
+  <si>
+    <t>TS_059</t>
+  </si>
+  <si>
+    <t>TS_060</t>
+  </si>
+  <si>
+    <t>TS_061</t>
+  </si>
+  <si>
+    <t>TS_062</t>
+  </si>
+  <si>
+    <t>TS_063</t>
+  </si>
+  <si>
+    <t>Waiting Quan Ly Cham Bai</t>
+  </si>
+  <si>
+    <t>quanLyChamBai_Tab</t>
+  </si>
+  <si>
+    <t>Click Quan Ly Cham Bai</t>
+  </si>
+  <si>
+    <t>Click Cham Bai</t>
+  </si>
+  <si>
+    <t>chamBai_Tab</t>
+  </si>
+  <si>
+    <t>TS_064</t>
+  </si>
+  <si>
+    <t>TS_065</t>
+  </si>
+  <si>
+    <t>TS_066</t>
+  </si>
+  <si>
     <t>PASS</t>
-  </si>
-  <si>
-    <t>Cource_Page</t>
   </si>
 </sst>
 </file>
@@ -950,7 +1112,7 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>161</v>
+        <v>216</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.45">
@@ -972,10 +1134,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A696EC6A-F50E-4D7B-ABB3-CDE9DA0E200A}">
-  <dimension ref="A1:I47"/>
+  <dimension ref="A1:K83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -987,7 +1149,7 @@
     <col min="7" max="7" customWidth="true" width="12.53125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1013,8 +1175,10 @@
         <v>3</v>
       </c>
       <c r="I1" s="3"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
         <v>152</v>
       </c>
@@ -1033,11 +1197,13 @@
         <v>72</v>
       </c>
       <c r="H2" t="s">
-        <v>161</v>
+        <v>216</v>
       </c>
       <c r="I2" s="3"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
         <v>152</v>
       </c>
@@ -1056,11 +1222,13 @@
         <v>149</v>
       </c>
       <c r="H3" t="s">
-        <v>161</v>
+        <v>216</v>
       </c>
       <c r="I3" s="3"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
         <v>152</v>
       </c>
@@ -1083,11 +1251,13 @@
         <v>90</v>
       </c>
       <c r="H4" t="s">
-        <v>161</v>
+        <v>216</v>
       </c>
       <c r="I4" s="3"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" s="3" t="s">
         <v>152</v>
       </c>
@@ -1108,11 +1278,13 @@
       </c>
       <c r="G5" s="5"/>
       <c r="H5" t="s">
-        <v>161</v>
+        <v>216</v>
       </c>
       <c r="I5" s="3"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
         <v>152</v>
       </c>
@@ -1133,11 +1305,13 @@
       </c>
       <c r="G6" s="4"/>
       <c r="H6" t="s">
-        <v>161</v>
+        <v>216</v>
       </c>
       <c r="I6" s="3"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
         <v>152</v>
       </c>
@@ -1160,11 +1334,13 @@
         <v>127</v>
       </c>
       <c r="H7" t="s">
-        <v>161</v>
+        <v>216</v>
       </c>
       <c r="I7" s="3"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
         <v>152</v>
       </c>
@@ -1187,11 +1363,13 @@
         <v>73</v>
       </c>
       <c r="H8" t="s">
-        <v>161</v>
+        <v>216</v>
       </c>
       <c r="I8" s="3"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A9" s="3" t="s">
         <v>152</v>
       </c>
@@ -1214,11 +1392,13 @@
         <v>38</v>
       </c>
       <c r="H9" t="s">
-        <v>161</v>
+        <v>216</v>
       </c>
       <c r="I9" s="3"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A10" s="3" t="s">
         <v>152</v>
       </c>
@@ -1239,11 +1419,13 @@
       </c>
       <c r="G10" s="5"/>
       <c r="H10" t="s">
-        <v>161</v>
+        <v>216</v>
       </c>
       <c r="I10" s="3"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A11" s="3" t="s">
         <v>152</v>
       </c>
@@ -1264,11 +1446,13 @@
       </c>
       <c r="G11" s="4"/>
       <c r="H11" t="s">
-        <v>161</v>
+        <v>216</v>
       </c>
       <c r="I11" s="3"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A12" s="3" t="s">
         <v>152</v>
       </c>
@@ -1291,11 +1475,13 @@
         <v>38</v>
       </c>
       <c r="H12" t="s">
-        <v>161</v>
+        <v>216</v>
       </c>
       <c r="I12" s="3"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A13" s="3" t="s">
         <v>152</v>
       </c>
@@ -1316,11 +1502,13 @@
       </c>
       <c r="G13" s="5"/>
       <c r="H13" t="s">
-        <v>161</v>
+        <v>216</v>
       </c>
       <c r="I13" s="3"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A14" s="3" t="s">
         <v>152</v>
       </c>
@@ -1343,11 +1531,13 @@
         <v>113</v>
       </c>
       <c r="H14" t="s">
-        <v>161</v>
+        <v>216</v>
       </c>
       <c r="I14" s="3"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A15" s="3" t="s">
         <v>152</v>
       </c>
@@ -1367,14 +1557,16 @@
         <v>37</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>38</v>
+        <v>183</v>
       </c>
       <c r="H15" t="s">
-        <v>161</v>
+        <v>216</v>
       </c>
       <c r="I15" s="3"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A16" s="3" t="s">
         <v>152</v>
       </c>
@@ -1397,11 +1589,13 @@
         <v>147</v>
       </c>
       <c r="H16" t="s">
-        <v>161</v>
+        <v>216</v>
       </c>
       <c r="I16" s="3"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A17" s="3" t="s">
         <v>152</v>
       </c>
@@ -1422,11 +1616,13 @@
       </c>
       <c r="G17" s="4"/>
       <c r="H17" t="s">
-        <v>161</v>
+        <v>216</v>
       </c>
       <c r="I17" s="3"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A18" s="3" t="s">
         <v>152</v>
       </c>
@@ -1437,7 +1633,7 @@
         <v>116</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>117</v>
@@ -1447,11 +1643,13 @@
       </c>
       <c r="G18" s="4"/>
       <c r="H18" t="s">
-        <v>161</v>
+        <v>216</v>
       </c>
       <c r="I18" s="3"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A19" s="3" t="s">
         <v>152</v>
       </c>
@@ -1462,7 +1660,7 @@
         <v>118</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>119</v>
@@ -1472,11 +1670,13 @@
       </c>
       <c r="G19" s="4"/>
       <c r="H19" t="s">
-        <v>161</v>
+        <v>216</v>
       </c>
       <c r="I19" s="3"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A20" s="3" t="s">
         <v>152</v>
       </c>
@@ -1487,7 +1687,7 @@
         <v>130</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>120</v>
@@ -1499,11 +1699,13 @@
         <v>38</v>
       </c>
       <c r="H20" t="s">
-        <v>161</v>
+        <v>216</v>
       </c>
       <c r="I20" s="3"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A21" s="3" t="s">
         <v>152</v>
       </c>
@@ -1514,7 +1716,7 @@
         <v>131</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>120</v>
@@ -1524,11 +1726,13 @@
       </c>
       <c r="G21" s="5"/>
       <c r="H21" t="s">
-        <v>161</v>
+        <v>216</v>
       </c>
       <c r="I21" s="3"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A22" s="3" t="s">
         <v>152</v>
       </c>
@@ -1539,7 +1743,7 @@
         <v>137</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>136</v>
@@ -1549,11 +1753,13 @@
       </c>
       <c r="G22" s="5"/>
       <c r="H22" t="s">
-        <v>161</v>
+        <v>216</v>
       </c>
       <c r="I22" s="3"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A23" s="3" t="s">
         <v>152</v>
       </c>
@@ -1564,7 +1770,7 @@
         <v>144</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>143</v>
@@ -1574,11 +1780,13 @@
       </c>
       <c r="G23" s="5"/>
       <c r="H23" t="s">
-        <v>161</v>
+        <v>216</v>
       </c>
       <c r="I23" s="3"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A24" s="3" t="s">
         <v>152</v>
       </c>
@@ -1589,7 +1797,7 @@
         <v>145</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>148</v>
@@ -1599,11 +1807,13 @@
       </c>
       <c r="G24" s="5"/>
       <c r="H24" t="s">
-        <v>161</v>
+        <v>216</v>
       </c>
       <c r="I24" s="3"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A25" s="3" t="s">
         <v>152</v>
       </c>
@@ -1614,7 +1824,7 @@
         <v>133</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>132</v>
@@ -1624,11 +1834,13 @@
       </c>
       <c r="G25" s="5"/>
       <c r="H25" t="s">
-        <v>161</v>
+        <v>216</v>
       </c>
       <c r="I25" s="3"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A26" s="3" t="s">
         <v>152</v>
       </c>
@@ -1639,7 +1851,7 @@
         <v>134</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>119</v>
@@ -1649,11 +1861,13 @@
       </c>
       <c r="G26" s="5"/>
       <c r="H26" t="s">
-        <v>161</v>
+        <v>216</v>
       </c>
       <c r="I26" s="3"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A27" s="3" t="s">
         <v>152</v>
       </c>
@@ -1664,7 +1878,7 @@
         <v>155</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>154</v>
@@ -1674,11 +1888,13 @@
       </c>
       <c r="G27" s="5"/>
       <c r="H27" t="s">
-        <v>161</v>
+        <v>216</v>
       </c>
       <c r="I27" s="3"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A28" s="3" t="s">
         <v>152</v>
       </c>
@@ -1699,11 +1915,13 @@
       </c>
       <c r="G28" s="5"/>
       <c r="H28" t="s">
-        <v>161</v>
+        <v>216</v>
       </c>
       <c r="I28" s="3"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A29" s="3" t="s">
         <v>152</v>
       </c>
@@ -1711,124 +1929,148 @@
         <v>88</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
+        <v>162</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>163</v>
+      </c>
       <c r="F29" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="G29" s="3"/>
+        <v>28</v>
+      </c>
+      <c r="G29" s="5"/>
       <c r="H29" t="s">
-        <v>161</v>
+        <v>216</v>
       </c>
       <c r="I29" s="3"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J29" s="3"/>
+      <c r="K29" s="3"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A30" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>98</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
+        <v>164</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>165</v>
+      </c>
       <c r="F30" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G30" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="H30" s="3"/>
+        <v>28</v>
+      </c>
+      <c r="G30" s="5"/>
+      <c r="H30" t="s">
+        <v>216</v>
+      </c>
       <c r="I30" s="3"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J30" s="3"/>
+      <c r="K30" s="3"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A31" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>103</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
+        <v>166</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>167</v>
+      </c>
       <c r="F31" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G31" s="4"/>
-      <c r="H31" s="3"/>
+        <v>28</v>
+      </c>
+      <c r="G31" s="5"/>
+      <c r="H31" t="s">
+        <v>216</v>
+      </c>
       <c r="I31" s="3"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J31" s="3"/>
+      <c r="K31" s="3"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A32" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>107</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>17</v>
+        <v>179</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>59</v>
+        <v>161</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>19</v>
+        <v>168</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G32" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="H32" s="3"/>
+        <v>28</v>
+      </c>
+      <c r="G32" s="5"/>
+      <c r="H32" t="s">
+        <v>216</v>
+      </c>
       <c r="I32" s="3"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J32" s="3"/>
+      <c r="K32" s="3"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A33" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>121</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>23</v>
+        <v>169</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>18</v>
+        <v>161</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>24</v>
+        <v>170</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G33" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="H33" s="3"/>
+        <v>28</v>
+      </c>
+      <c r="G33" s="5"/>
+      <c r="H33" t="s">
+        <v>216</v>
+      </c>
       <c r="I33" s="3"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J33" s="3"/>
+      <c r="K33" s="3"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A34" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>122</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>70</v>
+        <v>180</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>18</v>
+        <v>161</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>27</v>
+        <v>171</v>
       </c>
       <c r="F34" s="3" t="s">
         <v>37</v>
@@ -1836,278 +2078,1100 @@
       <c r="G34" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="H34" s="3"/>
+      <c r="H34" t="s">
+        <v>216</v>
+      </c>
       <c r="I34" s="3"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J34" s="3"/>
+      <c r="K34" s="3"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A35" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>123</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>71</v>
+        <v>178</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>18</v>
+        <v>161</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>27</v>
+        <v>171</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="G35" s="5"/>
-      <c r="H35" s="3"/>
+      <c r="H35" t="s">
+        <v>216</v>
+      </c>
       <c r="I35" s="3"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J35" s="3"/>
+      <c r="K35" s="3"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A36" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>124</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>26</v>
+        <v>186</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>18</v>
+        <v>161</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>27</v>
+        <v>173</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G36" s="4"/>
-      <c r="H36" s="3"/>
+        <v>37</v>
+      </c>
+      <c r="G36" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H36" t="s">
+        <v>216</v>
+      </c>
       <c r="I36" s="3"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J36" s="3"/>
+      <c r="K36" s="3"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A37" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>125</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>69</v>
+        <v>172</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>34</v>
+        <v>161</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>56</v>
+        <v>173</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>68</v>
+        <v>20</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="H37" s="3"/>
+        <v>174</v>
+      </c>
+      <c r="H37" t="s">
+        <v>216</v>
+      </c>
       <c r="I37" s="3"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J37" s="3"/>
+      <c r="K37" s="3"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A38" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>138</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>29</v>
+        <v>175</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>34</v>
+        <v>161</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>30</v>
+        <v>176</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G38" s="4"/>
-      <c r="H38" s="3"/>
+        <v>28</v>
+      </c>
+      <c r="G38" s="5"/>
+      <c r="H38" t="s">
+        <v>216</v>
+      </c>
       <c r="I38" s="3"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J38" s="3"/>
+      <c r="K38" s="3"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A39" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>139</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>33</v>
+        <v>184</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>34</v>
+        <v>161</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>30</v>
+        <v>185</v>
       </c>
       <c r="F39" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G39" s="4"/>
-      <c r="H39" s="3"/>
+      <c r="G39" s="5"/>
+      <c r="H39" t="s">
+        <v>216</v>
+      </c>
       <c r="I39" s="3"/>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J39" s="3"/>
+      <c r="K39" s="3"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A40" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>140</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>61</v>
+        <v>181</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>34</v>
+        <v>161</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>36</v>
+        <v>182</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="G40" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="H40" s="3"/>
+        <v>28</v>
+      </c>
+      <c r="G40" s="5"/>
+      <c r="H40" t="s">
+        <v>216</v>
+      </c>
       <c r="I40" s="3"/>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J40" s="3"/>
+      <c r="K40" s="3"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A41" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>141</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>36</v>
+        <v>76</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G41" s="4"/>
-      <c r="H41" s="3"/>
+        <v>37</v>
+      </c>
+      <c r="G41" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="H41" t="s">
+        <v>216</v>
+      </c>
       <c r="I41" s="3"/>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J41" s="3"/>
+      <c r="K41" s="3"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A42" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>158</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>36</v>
+        <v>76</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G42" s="4"/>
-      <c r="H42" s="3"/>
+        <v>31</v>
+      </c>
+      <c r="G42" s="5"/>
+      <c r="H42" t="s">
+        <v>216</v>
+      </c>
       <c r="I42" s="3"/>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J42" s="3"/>
+      <c r="K42" s="3"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A43" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>159</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>60</v>
+        <v>76</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="G43" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="H43" s="3"/>
+        <v>28</v>
+      </c>
+      <c r="G43" s="4"/>
+      <c r="H43" t="s">
+        <v>216</v>
+      </c>
       <c r="I43" s="3"/>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J43" s="3"/>
+      <c r="K43" s="3"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A44" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>160</v>
       </c>
       <c r="C44" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="H44" t="s">
+        <v>216</v>
+      </c>
+      <c r="I44" s="3"/>
+      <c r="J44" s="3"/>
+      <c r="K44" s="3"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A45" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G45" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H45" t="s">
+        <v>216</v>
+      </c>
+      <c r="I45" s="3"/>
+      <c r="J45" s="3"/>
+      <c r="K45" s="3"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A46" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G46" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H46" t="s">
+        <v>216</v>
+      </c>
+      <c r="I46" s="3"/>
+      <c r="J46" s="3"/>
+      <c r="K46" s="3"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A47" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G47" s="5"/>
+      <c r="H47" t="s">
+        <v>216</v>
+      </c>
+      <c r="I47" s="3"/>
+      <c r="J47" s="3"/>
+      <c r="K47" s="3"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A48" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="F48" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G48" s="4"/>
+      <c r="H48" t="s">
+        <v>216</v>
+      </c>
+      <c r="I48" s="3"/>
+      <c r="J48" s="3"/>
+      <c r="K48" s="3"/>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A49" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="F49" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G49" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H49" t="s">
+        <v>216</v>
+      </c>
+      <c r="I49" s="3"/>
+      <c r="J49" s="3"/>
+      <c r="K49" s="3"/>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A50" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="F50" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G50" s="5"/>
+      <c r="H50" t="s">
+        <v>216</v>
+      </c>
+      <c r="I50" s="3"/>
+      <c r="J50" s="3"/>
+      <c r="K50" s="3"/>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A51" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="F51" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G51" s="5"/>
+      <c r="H51" t="s">
+        <v>216</v>
+      </c>
+      <c r="I51" s="3"/>
+      <c r="J51" s="3"/>
+      <c r="K51" s="3"/>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A52" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="C52" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D44" s="3"/>
-      <c r="E44" s="3"/>
-      <c r="F44" s="3" t="s">
+      <c r="D52" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="E52" s="3"/>
+      <c r="F52" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="G44" s="3"/>
-      <c r="H44" s="3"/>
-      <c r="I44" s="3"/>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A45" s="3"/>
-      <c r="B45" s="3"/>
-      <c r="C45" s="3"/>
-      <c r="D45" s="3"/>
-      <c r="E45" s="3"/>
-      <c r="F45" s="3"/>
-      <c r="G45" s="3"/>
-      <c r="H45" s="3"/>
-      <c r="I45" s="3"/>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A46" s="3"/>
-      <c r="B46" s="3"/>
-      <c r="C46" s="3"/>
-      <c r="D46" s="3"/>
-      <c r="E46" s="3"/>
-      <c r="F46" s="3"/>
-      <c r="G46" s="3"/>
-      <c r="H46" s="3"/>
-      <c r="I46" s="3"/>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A47" s="3"/>
-      <c r="B47" s="3"/>
-      <c r="C47" s="3"/>
-      <c r="D47" s="3"/>
-      <c r="E47" s="3"/>
-      <c r="F47" s="3"/>
-      <c r="G47" s="3"/>
-      <c r="H47" s="3"/>
-      <c r="I47" s="3"/>
+      <c r="G52" s="3"/>
+      <c r="H52" t="s">
+        <v>216</v>
+      </c>
+      <c r="I52" s="3"/>
+      <c r="J52" s="3"/>
+      <c r="K52" s="3"/>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A53" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D53" s="3"/>
+      <c r="E53" s="3"/>
+      <c r="F53" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G53" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="H53" s="3"/>
+      <c r="I53" s="3"/>
+      <c r="J53" s="3"/>
+      <c r="K53" s="3"/>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A54" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D54" s="3"/>
+      <c r="E54" s="3"/>
+      <c r="F54" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G54" s="4"/>
+      <c r="H54" s="3"/>
+      <c r="I54" s="3"/>
+      <c r="J54" s="3"/>
+      <c r="K54" s="3"/>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A55" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F55" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G55" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="H55" s="3"/>
+      <c r="I55" s="3"/>
+      <c r="J55" s="3"/>
+      <c r="K55" s="3"/>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A56" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F56" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G56" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="H56" s="3"/>
+      <c r="I56" s="3"/>
+      <c r="J56" s="3"/>
+      <c r="K56" s="3"/>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A57" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F57" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G57" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H57" s="3"/>
+      <c r="I57" s="3"/>
+      <c r="J57" s="3"/>
+      <c r="K57" s="3"/>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A58" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F58" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G58" s="5"/>
+      <c r="H58" s="3"/>
+      <c r="I58" s="3"/>
+      <c r="J58" s="3"/>
+      <c r="K58" s="3"/>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A59" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F59" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G59" s="4"/>
+      <c r="H59" s="3"/>
+      <c r="I59" s="3"/>
+      <c r="J59" s="3"/>
+      <c r="K59" s="3"/>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A60" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F60" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G60" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H60" s="3"/>
+      <c r="I60" s="3"/>
+      <c r="J60" s="3"/>
+      <c r="K60" s="3"/>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A61" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F61" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G61" s="4"/>
+      <c r="H61" s="3"/>
+      <c r="I61" s="3"/>
+      <c r="J61" s="3"/>
+      <c r="K61" s="3"/>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A62" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F62" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G62" s="4"/>
+      <c r="H62" s="3"/>
+      <c r="I62" s="3"/>
+      <c r="J62" s="3"/>
+      <c r="K62" s="3"/>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A63" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F63" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G63" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H63" s="3"/>
+      <c r="I63" s="3"/>
+      <c r="J63" s="3"/>
+      <c r="K63" s="3"/>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A64" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F64" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G64" s="4"/>
+      <c r="H64" s="3"/>
+      <c r="I64" s="3"/>
+      <c r="J64" s="3"/>
+      <c r="K64" s="3"/>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A65" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E65" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F65" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G65" s="4"/>
+      <c r="H65" s="3"/>
+      <c r="I65" s="3"/>
+      <c r="J65" s="3"/>
+      <c r="K65" s="3"/>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A66" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E66" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F66" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G66" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="H66" s="3"/>
+      <c r="I66" s="3"/>
+      <c r="J66" s="3"/>
+      <c r="K66" s="3"/>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A67" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D67" s="3"/>
+      <c r="E67" s="3"/>
+      <c r="F67" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G67" s="3"/>
+      <c r="H67" s="3"/>
+      <c r="I67" s="3"/>
+      <c r="J67" s="3"/>
+      <c r="K67" s="3"/>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A68" s="3"/>
+      <c r="B68" s="3"/>
+      <c r="C68" s="3"/>
+      <c r="D68" s="3"/>
+      <c r="E68" s="3"/>
+      <c r="F68" s="3"/>
+      <c r="G68" s="3"/>
+      <c r="H68" s="3"/>
+      <c r="I68" s="3"/>
+      <c r="J68" s="3"/>
+      <c r="K68" s="3"/>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A69" s="3"/>
+      <c r="B69" s="3"/>
+      <c r="C69" s="3"/>
+      <c r="D69" s="3"/>
+      <c r="E69" s="3"/>
+      <c r="F69" s="3"/>
+      <c r="G69" s="3"/>
+      <c r="H69" s="3"/>
+      <c r="I69" s="3"/>
+      <c r="J69" s="3"/>
+      <c r="K69" s="3"/>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A70" s="3"/>
+      <c r="B70" s="3"/>
+      <c r="C70" s="3"/>
+      <c r="D70" s="3"/>
+      <c r="E70" s="3"/>
+      <c r="F70" s="3"/>
+      <c r="G70" s="3"/>
+      <c r="H70" s="3"/>
+      <c r="I70" s="3"/>
+      <c r="J70" s="3"/>
+      <c r="K70" s="3"/>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A71" s="3"/>
+      <c r="B71" s="3"/>
+      <c r="C71" s="3"/>
+      <c r="D71" s="3"/>
+      <c r="E71" s="3"/>
+      <c r="F71" s="3"/>
+      <c r="G71" s="3"/>
+      <c r="H71" s="3"/>
+      <c r="I71" s="3"/>
+      <c r="J71" s="3"/>
+      <c r="K71" s="3"/>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A72" s="3"/>
+      <c r="B72" s="3"/>
+      <c r="C72" s="3"/>
+      <c r="D72" s="3"/>
+      <c r="E72" s="3"/>
+      <c r="F72" s="3"/>
+      <c r="G72" s="3"/>
+      <c r="H72" s="3"/>
+      <c r="I72" s="3"/>
+      <c r="J72" s="3"/>
+      <c r="K72" s="3"/>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A73" s="3"/>
+      <c r="B73" s="3"/>
+      <c r="C73" s="3"/>
+      <c r="D73" s="3"/>
+      <c r="E73" s="3"/>
+      <c r="F73" s="3"/>
+      <c r="G73" s="3"/>
+      <c r="H73" s="3"/>
+      <c r="I73" s="3"/>
+      <c r="J73" s="3"/>
+      <c r="K73" s="3"/>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A74" s="3"/>
+      <c r="B74" s="3"/>
+      <c r="C74" s="3"/>
+      <c r="D74" s="3"/>
+      <c r="E74" s="3"/>
+      <c r="F74" s="3"/>
+      <c r="G74" s="3"/>
+      <c r="H74" s="3"/>
+      <c r="I74" s="3"/>
+      <c r="J74" s="3"/>
+      <c r="K74" s="3"/>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A75" s="3"/>
+      <c r="B75" s="3"/>
+      <c r="C75" s="3"/>
+      <c r="D75" s="3"/>
+      <c r="E75" s="3"/>
+      <c r="F75" s="3"/>
+      <c r="G75" s="3"/>
+      <c r="H75" s="3"/>
+      <c r="I75" s="3"/>
+      <c r="J75" s="3"/>
+      <c r="K75" s="3"/>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A76" s="3"/>
+      <c r="B76" s="3"/>
+      <c r="C76" s="3"/>
+      <c r="D76" s="3"/>
+      <c r="E76" s="3"/>
+      <c r="F76" s="3"/>
+      <c r="G76" s="3"/>
+      <c r="H76" s="3"/>
+      <c r="I76" s="3"/>
+      <c r="J76" s="3"/>
+      <c r="K76" s="3"/>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A77" s="3"/>
+      <c r="B77" s="3"/>
+      <c r="C77" s="3"/>
+      <c r="D77" s="3"/>
+      <c r="E77" s="3"/>
+      <c r="F77" s="3"/>
+      <c r="G77" s="3"/>
+      <c r="H77" s="3"/>
+      <c r="I77" s="3"/>
+      <c r="J77" s="3"/>
+      <c r="K77" s="3"/>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A78" s="3"/>
+      <c r="B78" s="3"/>
+      <c r="C78" s="3"/>
+      <c r="D78" s="3"/>
+      <c r="E78" s="3"/>
+      <c r="F78" s="3"/>
+      <c r="G78" s="3"/>
+      <c r="H78" s="3"/>
+      <c r="I78" s="3"/>
+      <c r="J78" s="3"/>
+      <c r="K78" s="3"/>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A79" s="3"/>
+      <c r="B79" s="3"/>
+      <c r="C79" s="3"/>
+      <c r="D79" s="3"/>
+      <c r="E79" s="3"/>
+      <c r="F79" s="3"/>
+      <c r="G79" s="3"/>
+      <c r="H79" s="3"/>
+      <c r="I79" s="3"/>
+      <c r="J79" s="3"/>
+      <c r="K79" s="3"/>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A80" s="3"/>
+      <c r="B80" s="3"/>
+      <c r="C80" s="3"/>
+      <c r="D80" s="3"/>
+      <c r="E80" s="3"/>
+      <c r="F80" s="3"/>
+      <c r="G80" s="3"/>
+      <c r="H80" s="3"/>
+      <c r="I80" s="3"/>
+      <c r="J80" s="3"/>
+      <c r="K80" s="3"/>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A81" s="3"/>
+      <c r="B81" s="3"/>
+      <c r="C81" s="3"/>
+      <c r="D81" s="3"/>
+      <c r="E81" s="3"/>
+      <c r="F81" s="3"/>
+      <c r="G81" s="3"/>
+      <c r="H81" s="3"/>
+      <c r="I81" s="3"/>
+      <c r="J81" s="3"/>
+      <c r="K81" s="3"/>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A82" s="3"/>
+      <c r="B82" s="3"/>
+      <c r="C82" s="3"/>
+      <c r="D82" s="3"/>
+      <c r="E82" s="3"/>
+      <c r="F82" s="3"/>
+      <c r="G82" s="3"/>
+      <c r="H82" s="3"/>
+      <c r="I82" s="3"/>
+      <c r="J82" s="3"/>
+      <c r="K82" s="3"/>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A83" s="3"/>
+      <c r="B83" s="3"/>
+      <c r="C83" s="3"/>
+      <c r="D83" s="3"/>
+      <c r="E83" s="3"/>
+      <c r="F83" s="3"/>
+      <c r="G83" s="3"/>
+      <c r="H83" s="3"/>
+      <c r="I83" s="3"/>
+      <c r="J83" s="3"/>
+      <c r="K83" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D44" xr:uid="{710BACEF-CE5A-4C56-B5C5-5E1AC5E70F66}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D67" xr:uid="{710BACEF-CE5A-4C56-B5C5-5E1AC5E70F66}">
       <formula1>Page_Name</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F1048576" xr:uid="{8405667A-AA8D-489C-B5B3-B6EA9D6474AC}">
@@ -2117,9 +3181,10 @@
   <hyperlinks>
     <hyperlink ref="G7" r:id="rId1" xr:uid="{A037A5DD-8D7E-4EB7-8B48-DAD212B537F3}"/>
     <hyperlink ref="G3" r:id="rId2" xr:uid="{42283EFE-4D4F-49BA-A138-E02C3F803720}"/>
+    <hyperlink ref="G44" r:id="rId3" xr:uid="{FB3B981E-F9DD-4E1C-9770-293AC7C73B6C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -2187,10 +3252,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E039E608-272C-4340-A7D2-E2A9089EF229}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2252,7 +3317,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B4" t="s">
         <v>51</v>
@@ -2386,6 +3451,46 @@
     <row r="21" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B21" t="s">
         <v>156</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B22" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B23" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B24" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B25" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B26" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B27" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B28" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B29" t="s">
+        <v>209</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update step verify result bai thuc hanh success
</commit_message>
<xml_diff>
--- a/src/test/java/dataEngine/DataEngine.xlsx
+++ b/src/test/java/dataEngine/DataEngine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Automation\working\SendID\senid\src\test\java\dataEngine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A20CC206-D7FD-41E5-B628-E5E6A3F62166}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9578762B-1A34-4FE4-81AE-66403164A03B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="1650" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{81D78742-11F9-4B4A-A9D3-448BFA7463DC}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1027" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="969" uniqueCount="341">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -1011,67 +1011,67 @@
     <t>TS_114</t>
   </si>
   <si>
+    <t xml:space="preserve">Click on answer "Kiem Tra Cuoi Khoa" </t>
+  </si>
+  <si>
+    <t>answerKiemTraCuoiKhoa</t>
+  </si>
+  <si>
+    <t>Verify "So Lan Lam Lai Bai Kiem Tra"</t>
+  </si>
+  <si>
+    <t>Wait for "Giai Thich"</t>
+  </si>
+  <si>
+    <t>giaiThich_Text</t>
+  </si>
+  <si>
+    <t>Verify content "Giai Thich"</t>
+  </si>
+  <si>
+    <t>Verify content "Giai Thich Cua Giao Vien"</t>
+  </si>
+  <si>
+    <t>giaiThichGiaoVien_Text</t>
+  </si>
+  <si>
+    <t>Verify result assingment</t>
+  </si>
+  <si>
+    <t>resultEssay</t>
+  </si>
+  <si>
+    <t>Dung</t>
+  </si>
+  <si>
+    <t>TS_115</t>
+  </si>
+  <si>
+    <t>TS_116</t>
+  </si>
+  <si>
+    <t>TS_117</t>
+  </si>
+  <si>
+    <t>TS_118</t>
+  </si>
+  <si>
+    <t>TS_119</t>
+  </si>
+  <si>
+    <t>TS_120</t>
+  </si>
+  <si>
+    <t>TS_121</t>
+  </si>
+  <si>
+    <t>FAIL</t>
+  </si>
+  <si>
+    <t>Mong muon cua em doi voi ngoi nha cua minh la gi?</t>
+  </si>
+  <si>
     <t>PASS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Click on answer "Kiem Tra Cuoi Khoa" </t>
-  </si>
-  <si>
-    <t>answerKiemTraCuoiKhoa</t>
-  </si>
-  <si>
-    <t>Verify "So Lan Lam Lai Bai Kiem Tra"</t>
-  </si>
-  <si>
-    <t>Wait for "Giai Thich"</t>
-  </si>
-  <si>
-    <t>giaiThich_Text</t>
-  </si>
-  <si>
-    <t>Verify content "Giai Thich"</t>
-  </si>
-  <si>
-    <t>Mong muon cua em doi voi ngoi nha</t>
-  </si>
-  <si>
-    <t>Verify content "Giai Thich Cua Giao Vien"</t>
-  </si>
-  <si>
-    <t>giaiThichGiaoVien_Text</t>
-  </si>
-  <si>
-    <t>Verify result assingment</t>
-  </si>
-  <si>
-    <t>resultEssay</t>
-  </si>
-  <si>
-    <t>Dung</t>
-  </si>
-  <si>
-    <t>TS_115</t>
-  </si>
-  <si>
-    <t>TS_116</t>
-  </si>
-  <si>
-    <t>TS_117</t>
-  </si>
-  <si>
-    <t>TS_118</t>
-  </si>
-  <si>
-    <t>TS_119</t>
-  </si>
-  <si>
-    <t>TS_120</t>
-  </si>
-  <si>
-    <t>TS_121</t>
-  </si>
-  <si>
-    <t>FAIL</t>
   </si>
 </sst>
 </file>
@@ -1512,10 +1512,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A696EC6A-F50E-4D7B-ABB3-CDE9DA0E200A}">
-  <dimension ref="A1:O143"/>
+  <dimension ref="A1:N134"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R14" sqref="R14"/>
+      <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1527,7 +1527,7 @@
     <col min="7" max="7" customWidth="true" width="12.53125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1558,9 +1558,8 @@
       <c r="L1" s="4"/>
       <c r="M1" s="4"/>
       <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A2" s="4" t="s">
         <v>150</v>
       </c>
@@ -1579,7 +1578,7 @@
         <v>71</v>
       </c>
       <c r="H2" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
@@ -1587,9 +1586,8 @@
       <c r="L2" s="4"/>
       <c r="M2" s="4"/>
       <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>150</v>
       </c>
@@ -1608,7 +1606,7 @@
         <v>148</v>
       </c>
       <c r="H3" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
@@ -1616,9 +1614,8 @@
       <c r="L3" s="4"/>
       <c r="M3" s="4"/>
       <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>150</v>
       </c>
@@ -1641,7 +1638,7 @@
         <v>89</v>
       </c>
       <c r="H4" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
@@ -1649,9 +1646,8 @@
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
       <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>150</v>
       </c>
@@ -1672,7 +1668,7 @@
       </c>
       <c r="G5" s="6"/>
       <c r="H5" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
@@ -1680,9 +1676,8 @@
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
       <c r="N5" s="4"/>
-      <c r="O5" s="4"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>150</v>
       </c>
@@ -1703,7 +1698,7 @@
       </c>
       <c r="G6" s="5"/>
       <c r="H6" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
@@ -1711,9 +1706,8 @@
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
       <c r="N6" s="4"/>
-      <c r="O6" s="4"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A7" s="4" t="s">
         <v>150</v>
       </c>
@@ -1736,7 +1730,7 @@
         <v>126</v>
       </c>
       <c r="H7" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
@@ -1744,9 +1738,8 @@
       <c r="L7" s="4"/>
       <c r="M7" s="4"/>
       <c r="N7" s="4"/>
-      <c r="O7" s="4"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A8" s="4" t="s">
         <v>150</v>
       </c>
@@ -1769,7 +1762,7 @@
         <v>72</v>
       </c>
       <c r="H8" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
@@ -1777,9 +1770,8 @@
       <c r="L8" s="4"/>
       <c r="M8" s="4"/>
       <c r="N8" s="4"/>
-      <c r="O8" s="4"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A9" s="4" t="s">
         <v>150</v>
       </c>
@@ -1802,7 +1794,7 @@
         <v>37</v>
       </c>
       <c r="H9" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
@@ -1810,9 +1802,8 @@
       <c r="L9" s="4"/>
       <c r="M9" s="4"/>
       <c r="N9" s="4"/>
-      <c r="O9" s="4"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A10" s="4" t="s">
         <v>150</v>
       </c>
@@ -1833,7 +1824,7 @@
       </c>
       <c r="G10" s="6"/>
       <c r="H10" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
@@ -1841,9 +1832,8 @@
       <c r="L10" s="4"/>
       <c r="M10" s="4"/>
       <c r="N10" s="4"/>
-      <c r="O10" s="4"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A11" s="4" t="s">
         <v>150</v>
       </c>
@@ -1864,7 +1854,7 @@
       </c>
       <c r="G11" s="5"/>
       <c r="H11" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
@@ -1872,9 +1862,8 @@
       <c r="L11" s="4"/>
       <c r="M11" s="4"/>
       <c r="N11" s="4"/>
-      <c r="O11" s="4"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A12" s="4" t="s">
         <v>150</v>
       </c>
@@ -1897,7 +1886,7 @@
         <v>37</v>
       </c>
       <c r="H12" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
@@ -1905,9 +1894,8 @@
       <c r="L12" s="4"/>
       <c r="M12" s="4"/>
       <c r="N12" s="4"/>
-      <c r="O12" s="4"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A13" s="4" t="s">
         <v>150</v>
       </c>
@@ -1928,7 +1916,7 @@
       </c>
       <c r="G13" s="6"/>
       <c r="H13" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
@@ -1936,9 +1924,8 @@
       <c r="L13" s="4"/>
       <c r="M13" s="4"/>
       <c r="N13" s="4"/>
-      <c r="O13" s="4"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A14" s="4" t="s">
         <v>150</v>
       </c>
@@ -1961,7 +1948,7 @@
         <v>112</v>
       </c>
       <c r="H14" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
@@ -1969,9 +1956,8 @@
       <c r="L14" s="4"/>
       <c r="M14" s="4"/>
       <c r="N14" s="4"/>
-      <c r="O14" s="4"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A15" s="4" t="s">
         <v>150</v>
       </c>
@@ -1994,7 +1980,7 @@
         <v>89</v>
       </c>
       <c r="H15" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
@@ -2002,9 +1988,8 @@
       <c r="L15" s="4"/>
       <c r="M15" s="4"/>
       <c r="N15" s="4"/>
-      <c r="O15" s="4"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A16" s="4" t="s">
         <v>150</v>
       </c>
@@ -2027,7 +2012,7 @@
         <v>146</v>
       </c>
       <c r="H16" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
@@ -2035,9 +2020,8 @@
       <c r="L16" s="4"/>
       <c r="M16" s="4"/>
       <c r="N16" s="4"/>
-      <c r="O16" s="4"/>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A17" s="4" t="s">
         <v>150</v>
       </c>
@@ -2058,7 +2042,7 @@
       </c>
       <c r="G17" s="5"/>
       <c r="H17" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
@@ -2066,9 +2050,8 @@
       <c r="L17" s="4"/>
       <c r="M17" s="4"/>
       <c r="N17" s="4"/>
-      <c r="O17" s="4"/>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A18" s="4" t="s">
         <v>150</v>
       </c>
@@ -2089,7 +2072,7 @@
       </c>
       <c r="G18" s="5"/>
       <c r="H18" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I18" s="4"/>
       <c r="J18" s="4"/>
@@ -2097,9 +2080,8 @@
       <c r="L18" s="4"/>
       <c r="M18" s="4"/>
       <c r="N18" s="4"/>
-      <c r="O18" s="4"/>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A19" s="4" t="s">
         <v>150</v>
       </c>
@@ -2120,7 +2102,7 @@
       </c>
       <c r="G19" s="5"/>
       <c r="H19" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I19" s="4"/>
       <c r="J19" s="4"/>
@@ -2128,9 +2110,8 @@
       <c r="L19" s="4"/>
       <c r="M19" s="4"/>
       <c r="N19" s="4"/>
-      <c r="O19" s="4"/>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A20" s="4" t="s">
         <v>150</v>
       </c>
@@ -2153,7 +2134,7 @@
         <v>37</v>
       </c>
       <c r="H20" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
@@ -2161,9 +2142,8 @@
       <c r="L20" s="4"/>
       <c r="M20" s="4"/>
       <c r="N20" s="4"/>
-      <c r="O20" s="4"/>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A21" s="4" t="s">
         <v>150</v>
       </c>
@@ -2184,7 +2164,7 @@
       </c>
       <c r="G21" s="6"/>
       <c r="H21" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I21" s="4"/>
       <c r="J21" s="4"/>
@@ -2192,9 +2172,8 @@
       <c r="L21" s="4"/>
       <c r="M21" s="4"/>
       <c r="N21" s="4"/>
-      <c r="O21" s="4"/>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A22" s="4" t="s">
         <v>150</v>
       </c>
@@ -2215,7 +2194,7 @@
       </c>
       <c r="G22" s="6"/>
       <c r="H22" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
@@ -2223,9 +2202,8 @@
       <c r="L22" s="4"/>
       <c r="M22" s="4"/>
       <c r="N22" s="4"/>
-      <c r="O22" s="4"/>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A23" s="4" t="s">
         <v>150</v>
       </c>
@@ -2246,7 +2224,7 @@
       </c>
       <c r="G23" s="6"/>
       <c r="H23" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I23" s="4"/>
       <c r="J23" s="4"/>
@@ -2254,9 +2232,8 @@
       <c r="L23" s="4"/>
       <c r="M23" s="4"/>
       <c r="N23" s="4"/>
-      <c r="O23" s="4"/>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A24" s="4" t="s">
         <v>150</v>
       </c>
@@ -2277,7 +2254,7 @@
       </c>
       <c r="G24" s="6"/>
       <c r="H24" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I24" s="4"/>
       <c r="J24" s="4"/>
@@ -2285,9 +2262,8 @@
       <c r="L24" s="4"/>
       <c r="M24" s="4"/>
       <c r="N24" s="4"/>
-      <c r="O24" s="4"/>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A25" s="4" t="s">
         <v>150</v>
       </c>
@@ -2308,7 +2284,7 @@
       </c>
       <c r="G25" s="6"/>
       <c r="H25" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I25" s="4"/>
       <c r="J25" s="4"/>
@@ -2316,9 +2292,8 @@
       <c r="L25" s="4"/>
       <c r="M25" s="4"/>
       <c r="N25" s="4"/>
-      <c r="O25" s="4"/>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A26" s="4" t="s">
         <v>150</v>
       </c>
@@ -2339,7 +2314,7 @@
       </c>
       <c r="G26" s="6"/>
       <c r="H26" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I26" s="4"/>
       <c r="J26" s="4"/>
@@ -2347,9 +2322,8 @@
       <c r="L26" s="4"/>
       <c r="M26" s="4"/>
       <c r="N26" s="4"/>
-      <c r="O26" s="4"/>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A27" s="4" t="s">
         <v>150</v>
       </c>
@@ -2370,7 +2344,7 @@
       </c>
       <c r="G27" s="6"/>
       <c r="H27" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I27" s="4"/>
       <c r="J27" s="4"/>
@@ -2378,9 +2352,8 @@
       <c r="L27" s="4"/>
       <c r="M27" s="4"/>
       <c r="N27" s="4"/>
-      <c r="O27" s="4"/>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A28" s="4" t="s">
         <v>150</v>
       </c>
@@ -2401,7 +2374,7 @@
       </c>
       <c r="G28" s="6"/>
       <c r="H28" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I28" s="4"/>
       <c r="J28" s="4"/>
@@ -2409,9 +2382,8 @@
       <c r="L28" s="4"/>
       <c r="M28" s="4"/>
       <c r="N28" s="4"/>
-      <c r="O28" s="4"/>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A29" s="4" t="s">
         <v>150</v>
       </c>
@@ -2432,7 +2404,7 @@
       </c>
       <c r="G29" s="6"/>
       <c r="H29" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I29" s="4"/>
       <c r="J29" s="4"/>
@@ -2440,9 +2412,8 @@
       <c r="L29" s="4"/>
       <c r="M29" s="4"/>
       <c r="N29" s="4"/>
-      <c r="O29" s="4"/>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A30" s="4" t="s">
         <v>150</v>
       </c>
@@ -2463,7 +2434,7 @@
       </c>
       <c r="G30" s="6"/>
       <c r="H30" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I30" s="4"/>
       <c r="J30" s="4"/>
@@ -2471,9 +2442,8 @@
       <c r="L30" s="4"/>
       <c r="M30" s="4"/>
       <c r="N30" s="4"/>
-      <c r="O30" s="4"/>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A31" s="4" t="s">
         <v>150</v>
       </c>
@@ -2494,7 +2464,7 @@
       </c>
       <c r="G31" s="6"/>
       <c r="H31" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I31" s="4"/>
       <c r="J31" s="4"/>
@@ -2502,9 +2472,8 @@
       <c r="L31" s="4"/>
       <c r="M31" s="4"/>
       <c r="N31" s="4"/>
-      <c r="O31" s="4"/>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A32" s="4" t="s">
         <v>150</v>
       </c>
@@ -2525,7 +2494,7 @@
       </c>
       <c r="G32" s="6"/>
       <c r="H32" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I32" s="4"/>
       <c r="J32" s="4"/>
@@ -2533,9 +2502,8 @@
       <c r="L32" s="4"/>
       <c r="M32" s="4"/>
       <c r="N32" s="4"/>
-      <c r="O32" s="4"/>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A33" s="4" t="s">
         <v>150</v>
       </c>
@@ -2556,7 +2524,7 @@
       </c>
       <c r="G33" s="6"/>
       <c r="H33" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I33" s="4"/>
       <c r="J33" s="4"/>
@@ -2564,9 +2532,8 @@
       <c r="L33" s="4"/>
       <c r="M33" s="4"/>
       <c r="N33" s="4"/>
-      <c r="O33" s="4"/>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A34" s="4" t="s">
         <v>150</v>
       </c>
@@ -2589,7 +2556,7 @@
         <v>37</v>
       </c>
       <c r="H34" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I34" s="4"/>
       <c r="J34" s="4"/>
@@ -2597,9 +2564,8 @@
       <c r="L34" s="4"/>
       <c r="M34" s="4"/>
       <c r="N34" s="4"/>
-      <c r="O34" s="4"/>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A35" s="4" t="s">
         <v>150</v>
       </c>
@@ -2620,7 +2586,7 @@
       </c>
       <c r="G35" s="6"/>
       <c r="H35" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I35" s="4"/>
       <c r="J35" s="4"/>
@@ -2628,9 +2594,8 @@
       <c r="L35" s="4"/>
       <c r="M35" s="4"/>
       <c r="N35" s="4"/>
-      <c r="O35" s="4"/>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A36" s="4" t="s">
         <v>150</v>
       </c>
@@ -2651,7 +2616,7 @@
       </c>
       <c r="G36" s="6"/>
       <c r="H36" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I36" s="4"/>
       <c r="J36" s="4"/>
@@ -2659,9 +2624,8 @@
       <c r="L36" s="4"/>
       <c r="M36" s="4"/>
       <c r="N36" s="4"/>
-      <c r="O36" s="4"/>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A37" s="4" t="s">
         <v>150</v>
       </c>
@@ -2684,7 +2648,7 @@
         <v>37</v>
       </c>
       <c r="H37" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I37" s="4"/>
       <c r="J37" s="4"/>
@@ -2692,9 +2656,8 @@
       <c r="L37" s="4"/>
       <c r="M37" s="4"/>
       <c r="N37" s="4"/>
-      <c r="O37" s="4"/>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A38" s="4" t="s">
         <v>150</v>
       </c>
@@ -2717,7 +2680,7 @@
         <v>172</v>
       </c>
       <c r="H38" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I38" s="4"/>
       <c r="J38" s="4"/>
@@ -2725,9 +2688,8 @@
       <c r="L38" s="4"/>
       <c r="M38" s="4"/>
       <c r="N38" s="4"/>
-      <c r="O38" s="4"/>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A39" s="4" t="s">
         <v>150</v>
       </c>
@@ -2748,7 +2710,7 @@
       </c>
       <c r="G39" s="6"/>
       <c r="H39" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I39" s="4"/>
       <c r="J39" s="4"/>
@@ -2756,9 +2718,8 @@
       <c r="L39" s="4"/>
       <c r="M39" s="4"/>
       <c r="N39" s="4"/>
-      <c r="O39" s="4"/>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A40" s="4" t="s">
         <v>150</v>
       </c>
@@ -2781,7 +2742,7 @@
         <v>37</v>
       </c>
       <c r="H40" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I40" s="4"/>
       <c r="J40" s="4"/>
@@ -2789,9 +2750,8 @@
       <c r="L40" s="4"/>
       <c r="M40" s="4"/>
       <c r="N40" s="4"/>
-      <c r="O40" s="4"/>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A41" s="4" t="s">
         <v>150</v>
       </c>
@@ -2812,7 +2772,7 @@
       </c>
       <c r="G41" s="6"/>
       <c r="H41" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I41" s="4"/>
       <c r="J41" s="4"/>
@@ -2820,9 +2780,8 @@
       <c r="L41" s="4"/>
       <c r="M41" s="4"/>
       <c r="N41" s="4"/>
-      <c r="O41" s="4"/>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A42" s="4" t="s">
         <v>150</v>
       </c>
@@ -2845,7 +2804,7 @@
         <v>37</v>
       </c>
       <c r="H42" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I42" s="4"/>
       <c r="J42" s="4"/>
@@ -2853,9 +2812,8 @@
       <c r="L42" s="4"/>
       <c r="M42" s="4"/>
       <c r="N42" s="4"/>
-      <c r="O42" s="4"/>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A43" s="4" t="s">
         <v>150</v>
       </c>
@@ -2876,7 +2834,7 @@
       </c>
       <c r="G43" s="6"/>
       <c r="H43" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I43" s="4"/>
       <c r="J43" s="4"/>
@@ -2884,9 +2842,8 @@
       <c r="L43" s="4"/>
       <c r="M43" s="4"/>
       <c r="N43" s="4"/>
-      <c r="O43" s="4"/>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A44" s="4" t="s">
         <v>150</v>
       </c>
@@ -2909,7 +2866,7 @@
         <v>89</v>
       </c>
       <c r="H44" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I44" s="4"/>
       <c r="J44" s="4"/>
@@ -2917,9 +2874,8 @@
       <c r="L44" s="4"/>
       <c r="M44" s="4"/>
       <c r="N44" s="4"/>
-      <c r="O44" s="4"/>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A45" s="4" t="s">
         <v>150</v>
       </c>
@@ -2940,7 +2896,7 @@
       </c>
       <c r="G45" s="6"/>
       <c r="H45" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I45" s="4"/>
       <c r="J45" s="4"/>
@@ -2948,9 +2904,8 @@
       <c r="L45" s="4"/>
       <c r="M45" s="4"/>
       <c r="N45" s="4"/>
-      <c r="O45" s="4"/>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A46" s="4" t="s">
         <v>150</v>
       </c>
@@ -2971,7 +2926,7 @@
       </c>
       <c r="G46" s="5"/>
       <c r="H46" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I46" s="4"/>
       <c r="J46" s="4"/>
@@ -2979,9 +2934,8 @@
       <c r="L46" s="4"/>
       <c r="M46" s="4"/>
       <c r="N46" s="4"/>
-      <c r="O46" s="4"/>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A47" s="4" t="s">
         <v>150</v>
       </c>
@@ -3004,7 +2958,7 @@
         <v>191</v>
       </c>
       <c r="H47" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I47" s="4"/>
       <c r="J47" s="4"/>
@@ -3012,9 +2966,8 @@
       <c r="L47" s="4"/>
       <c r="M47" s="4"/>
       <c r="N47" s="4"/>
-      <c r="O47" s="4"/>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A48" s="4" t="s">
         <v>150</v>
       </c>
@@ -3037,7 +2990,7 @@
         <v>72</v>
       </c>
       <c r="H48" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I48" s="4"/>
       <c r="J48" s="4"/>
@@ -3045,9 +2998,8 @@
       <c r="L48" s="4"/>
       <c r="M48" s="4"/>
       <c r="N48" s="4"/>
-      <c r="O48" s="4"/>
-    </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A49" s="4" t="s">
         <v>150</v>
       </c>
@@ -3070,7 +3022,7 @@
         <v>37</v>
       </c>
       <c r="H49" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I49" s="4"/>
       <c r="J49" s="4"/>
@@ -3078,9 +3030,8 @@
       <c r="L49" s="4"/>
       <c r="M49" s="4"/>
       <c r="N49" s="4"/>
-      <c r="O49" s="4"/>
-    </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A50" s="4" t="s">
         <v>150</v>
       </c>
@@ -3101,7 +3052,7 @@
       </c>
       <c r="G50" s="6"/>
       <c r="H50" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I50" s="4"/>
       <c r="J50" s="4"/>
@@ -3109,9 +3060,8 @@
       <c r="L50" s="4"/>
       <c r="M50" s="4"/>
       <c r="N50" s="4"/>
-      <c r="O50" s="4"/>
-    </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A51" s="4" t="s">
         <v>150</v>
       </c>
@@ -3132,7 +3082,7 @@
       </c>
       <c r="G51" s="5"/>
       <c r="H51" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I51" s="4"/>
       <c r="J51" s="4"/>
@@ -3140,9 +3090,8 @@
       <c r="L51" s="4"/>
       <c r="M51" s="4"/>
       <c r="N51" s="4"/>
-      <c r="O51" s="4"/>
-    </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A52" s="4" t="s">
         <v>150</v>
       </c>
@@ -3165,7 +3114,7 @@
         <v>37</v>
       </c>
       <c r="H52" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I52" s="4"/>
       <c r="J52" s="4"/>
@@ -3173,9 +3122,8 @@
       <c r="L52" s="4"/>
       <c r="M52" s="4"/>
       <c r="N52" s="4"/>
-      <c r="O52" s="4"/>
-    </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A53" s="4" t="s">
         <v>150</v>
       </c>
@@ -3196,7 +3144,7 @@
       </c>
       <c r="G53" s="6"/>
       <c r="H53" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I53" s="4"/>
       <c r="J53" s="4"/>
@@ -3204,9 +3152,8 @@
       <c r="L53" s="4"/>
       <c r="M53" s="4"/>
       <c r="N53" s="4"/>
-      <c r="O53" s="4"/>
-    </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A54" s="4" t="s">
         <v>150</v>
       </c>
@@ -3227,7 +3174,7 @@
       </c>
       <c r="G54" s="6"/>
       <c r="H54" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I54" s="4"/>
       <c r="J54" s="4"/>
@@ -3235,9 +3182,8 @@
       <c r="L54" s="4"/>
       <c r="M54" s="4"/>
       <c r="N54" s="4"/>
-      <c r="O54" s="4"/>
-    </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A55" s="4" t="s">
         <v>150</v>
       </c>
@@ -3258,7 +3204,7 @@
         <v>221</v>
       </c>
       <c r="H55" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I55" s="4"/>
       <c r="J55" s="4"/>
@@ -3266,9 +3212,8 @@
       <c r="L55" s="4"/>
       <c r="M55" s="4"/>
       <c r="N55" s="4"/>
-      <c r="O55" s="4"/>
-    </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A56" s="4" t="s">
         <v>150</v>
       </c>
@@ -3291,7 +3236,7 @@
         <v>37</v>
       </c>
       <c r="H56" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I56" s="4"/>
       <c r="J56" s="4"/>
@@ -3299,9 +3244,8 @@
       <c r="L56" s="4"/>
       <c r="M56" s="4"/>
       <c r="N56" s="4"/>
-      <c r="O56" s="4"/>
-    </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A57" s="4" t="s">
         <v>150</v>
       </c>
@@ -3324,7 +3268,7 @@
         <v>37</v>
       </c>
       <c r="H57" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I57" s="4"/>
       <c r="J57" s="4"/>
@@ -3332,9 +3276,8 @@
       <c r="L57" s="4"/>
       <c r="M57" s="4"/>
       <c r="N57" s="4"/>
-      <c r="O57" s="4"/>
-    </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A58" s="4" t="s">
         <v>150</v>
       </c>
@@ -3355,7 +3298,7 @@
       </c>
       <c r="G58" s="6"/>
       <c r="H58" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I58" s="4"/>
       <c r="J58" s="4"/>
@@ -3363,9 +3306,8 @@
       <c r="L58" s="4"/>
       <c r="M58" s="4"/>
       <c r="N58" s="4"/>
-      <c r="O58" s="4"/>
-    </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A59" s="4" t="s">
         <v>150</v>
       </c>
@@ -3388,7 +3330,7 @@
         <v>37</v>
       </c>
       <c r="H59" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I59" s="4"/>
       <c r="J59" s="4"/>
@@ -3396,9 +3338,8 @@
       <c r="L59" s="4"/>
       <c r="M59" s="4"/>
       <c r="N59" s="4"/>
-      <c r="O59" s="4"/>
-    </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A60" s="4" t="s">
         <v>150</v>
       </c>
@@ -3421,7 +3362,7 @@
         <v>270</v>
       </c>
       <c r="H60" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I60" s="4"/>
       <c r="J60" s="4"/>
@@ -3429,9 +3370,8 @@
       <c r="L60" s="4"/>
       <c r="M60" s="4"/>
       <c r="N60" s="4"/>
-      <c r="O60" s="4"/>
-    </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A61" s="4" t="s">
         <v>150</v>
       </c>
@@ -3454,7 +3394,7 @@
         <v>37</v>
       </c>
       <c r="H61" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I61" s="4"/>
       <c r="J61" s="4"/>
@@ -3462,9 +3402,8 @@
       <c r="L61" s="4"/>
       <c r="M61" s="4"/>
       <c r="N61" s="4"/>
-      <c r="O61" s="4"/>
-    </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A62" s="4" t="s">
         <v>150</v>
       </c>
@@ -3485,7 +3424,7 @@
       </c>
       <c r="G62" s="6"/>
       <c r="H62" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I62" s="4"/>
       <c r="J62" s="4"/>
@@ -3493,9 +3432,8 @@
       <c r="L62" s="4"/>
       <c r="M62" s="4"/>
       <c r="N62" s="4"/>
-      <c r="O62" s="4"/>
-    </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A63" s="4" t="s">
         <v>150</v>
       </c>
@@ -3518,7 +3456,7 @@
         <v>274</v>
       </c>
       <c r="H63" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I63" s="4"/>
       <c r="J63" s="4"/>
@@ -3526,9 +3464,8 @@
       <c r="L63" s="4"/>
       <c r="M63" s="4"/>
       <c r="N63" s="4"/>
-      <c r="O63" s="4"/>
-    </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A64" s="4" t="s">
         <v>150</v>
       </c>
@@ -3551,7 +3488,7 @@
         <v>274</v>
       </c>
       <c r="H64" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I64" s="4"/>
       <c r="J64" s="4"/>
@@ -3559,9 +3496,8 @@
       <c r="L64" s="4"/>
       <c r="M64" s="4"/>
       <c r="N64" s="4"/>
-      <c r="O64" s="4"/>
-    </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A65" s="4" t="s">
         <v>150</v>
       </c>
@@ -3584,7 +3520,7 @@
         <v>274</v>
       </c>
       <c r="H65" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I65" s="4"/>
       <c r="J65" s="4"/>
@@ -3592,9 +3528,8 @@
       <c r="L65" s="4"/>
       <c r="M65" s="4"/>
       <c r="N65" s="4"/>
-      <c r="O65" s="4"/>
-    </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A66" s="4" t="s">
         <v>150</v>
       </c>
@@ -3617,7 +3552,7 @@
         <v>274</v>
       </c>
       <c r="H66" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I66" s="4"/>
       <c r="J66" s="4"/>
@@ -3625,9 +3560,8 @@
       <c r="L66" s="4"/>
       <c r="M66" s="4"/>
       <c r="N66" s="4"/>
-      <c r="O66" s="4"/>
-    </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A67" s="4" t="s">
         <v>150</v>
       </c>
@@ -3648,7 +3582,7 @@
       </c>
       <c r="G67" s="6"/>
       <c r="H67" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I67" s="4"/>
       <c r="J67" s="4"/>
@@ -3656,9 +3590,8 @@
       <c r="L67" s="4"/>
       <c r="M67" s="4"/>
       <c r="N67" s="4"/>
-      <c r="O67" s="4"/>
-    </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A68" s="4" t="s">
         <v>150</v>
       </c>
@@ -3681,7 +3614,7 @@
         <v>37</v>
       </c>
       <c r="H68" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I68" s="4"/>
       <c r="J68" s="4"/>
@@ -3689,9 +3622,8 @@
       <c r="L68" s="4"/>
       <c r="M68" s="4"/>
       <c r="N68" s="4"/>
-      <c r="O68" s="4"/>
-    </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A69" s="4" t="s">
         <v>150</v>
       </c>
@@ -3714,7 +3646,7 @@
         <v>239</v>
       </c>
       <c r="H69" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I69" s="4"/>
       <c r="J69" s="4"/>
@@ -3722,9 +3654,8 @@
       <c r="L69" s="4"/>
       <c r="M69" s="4"/>
       <c r="N69" s="4"/>
-      <c r="O69" s="4"/>
-    </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A70" s="4" t="s">
         <v>150</v>
       </c>
@@ -3745,7 +3676,7 @@
       </c>
       <c r="G70" s="6"/>
       <c r="H70" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I70" s="4"/>
       <c r="J70" s="4"/>
@@ -3753,9 +3684,8 @@
       <c r="L70" s="4"/>
       <c r="M70" s="4"/>
       <c r="N70" s="4"/>
-      <c r="O70" s="4"/>
-    </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A71" s="4" t="s">
         <v>150</v>
       </c>
@@ -3776,7 +3706,7 @@
       </c>
       <c r="G71" s="6"/>
       <c r="H71" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I71" s="4"/>
       <c r="J71" s="4"/>
@@ -3784,9 +3714,8 @@
       <c r="L71" s="4"/>
       <c r="M71" s="4"/>
       <c r="N71" s="4"/>
-      <c r="O71" s="4"/>
-    </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A72" s="4" t="s">
         <v>150</v>
       </c>
@@ -3809,7 +3738,7 @@
         <v>37</v>
       </c>
       <c r="H72" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I72" s="4"/>
       <c r="J72" s="4"/>
@@ -3817,9 +3746,8 @@
       <c r="L72" s="4"/>
       <c r="M72" s="4"/>
       <c r="N72" s="4"/>
-      <c r="O72" s="4"/>
-    </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="73" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A73" s="4" t="s">
         <v>150</v>
       </c>
@@ -3842,7 +3770,7 @@
         <v>246</v>
       </c>
       <c r="H73" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I73" s="4"/>
       <c r="J73" s="4"/>
@@ -3850,9 +3778,8 @@
       <c r="L73" s="4"/>
       <c r="M73" s="4"/>
       <c r="N73" s="4"/>
-      <c r="O73" s="4"/>
-    </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="74" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A74" s="4" t="s">
         <v>150</v>
       </c>
@@ -3873,7 +3800,7 @@
       </c>
       <c r="G74" s="6"/>
       <c r="H74" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I74" s="4"/>
       <c r="J74" s="4"/>
@@ -3881,9 +3808,8 @@
       <c r="L74" s="4"/>
       <c r="M74" s="4"/>
       <c r="N74" s="4"/>
-      <c r="O74" s="4"/>
-    </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="75" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A75" s="4" t="s">
         <v>150</v>
       </c>
@@ -3906,7 +3832,7 @@
         <v>37</v>
       </c>
       <c r="H75" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I75" s="4"/>
       <c r="J75" s="4"/>
@@ -3914,9 +3840,8 @@
       <c r="L75" s="4"/>
       <c r="M75" s="4"/>
       <c r="N75" s="4"/>
-      <c r="O75" s="4"/>
-    </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="76" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A76" s="4" t="s">
         <v>150</v>
       </c>
@@ -3937,7 +3862,7 @@
       </c>
       <c r="G76" s="6"/>
       <c r="H76" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I76" s="4"/>
       <c r="J76" s="4"/>
@@ -3945,9 +3870,8 @@
       <c r="L76" s="4"/>
       <c r="M76" s="4"/>
       <c r="N76" s="4"/>
-      <c r="O76" s="4"/>
-    </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="77" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A77" s="4" t="s">
         <v>150</v>
       </c>
@@ -3968,7 +3892,7 @@
       </c>
       <c r="G77" s="6"/>
       <c r="H77" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I77" s="4"/>
       <c r="J77" s="4"/>
@@ -3976,9 +3900,8 @@
       <c r="L77" s="4"/>
       <c r="M77" s="4"/>
       <c r="N77" s="4"/>
-      <c r="O77" s="4"/>
-    </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="78" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A78" s="4" t="s">
         <v>150</v>
       </c>
@@ -4001,7 +3924,7 @@
         <v>89</v>
       </c>
       <c r="H78" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I78" s="4"/>
       <c r="J78" s="4"/>
@@ -4009,9 +3932,8 @@
       <c r="L78" s="4"/>
       <c r="M78" s="4"/>
       <c r="N78" s="4"/>
-      <c r="O78" s="4"/>
-    </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="79" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A79" s="4" t="s">
         <v>150</v>
       </c>
@@ -4032,7 +3954,7 @@
       </c>
       <c r="G79" s="6"/>
       <c r="H79" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I79" s="4"/>
       <c r="J79" s="4"/>
@@ -4040,9 +3962,8 @@
       <c r="L79" s="4"/>
       <c r="M79" s="4"/>
       <c r="N79" s="4"/>
-      <c r="O79" s="4"/>
-    </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="80" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A80" s="4" t="s">
         <v>150</v>
       </c>
@@ -4063,7 +3984,7 @@
       </c>
       <c r="G80" s="5"/>
       <c r="H80" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I80" s="4"/>
       <c r="J80" s="4"/>
@@ -4071,9 +3992,8 @@
       <c r="L80" s="4"/>
       <c r="M80" s="4"/>
       <c r="N80" s="4"/>
-      <c r="O80" s="4"/>
-    </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="81" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A81" s="4" t="s">
         <v>150</v>
       </c>
@@ -4096,7 +4016,7 @@
         <v>126</v>
       </c>
       <c r="H81" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I81" s="4"/>
       <c r="J81" s="4"/>
@@ -4104,9 +4024,8 @@
       <c r="L81" s="4"/>
       <c r="M81" s="4"/>
       <c r="N81" s="4"/>
-      <c r="O81" s="4"/>
-    </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="82" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A82" s="4" t="s">
         <v>150</v>
       </c>
@@ -4129,7 +4048,7 @@
         <v>72</v>
       </c>
       <c r="H82" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I82" s="4"/>
       <c r="J82" s="4"/>
@@ -4137,9 +4056,8 @@
       <c r="L82" s="4"/>
       <c r="M82" s="4"/>
       <c r="N82" s="4"/>
-      <c r="O82" s="4"/>
-    </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="83" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A83" s="4" t="s">
         <v>150</v>
       </c>
@@ -4162,7 +4080,7 @@
         <v>37</v>
       </c>
       <c r="H83" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I83" s="4"/>
       <c r="J83" s="4"/>
@@ -4170,9 +4088,8 @@
       <c r="L83" s="4"/>
       <c r="M83" s="4"/>
       <c r="N83" s="4"/>
-      <c r="O83" s="4"/>
-    </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="84" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A84" s="4" t="s">
         <v>150</v>
       </c>
@@ -4193,7 +4110,7 @@
       </c>
       <c r="G84" s="6"/>
       <c r="H84" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I84" s="4"/>
       <c r="J84" s="4"/>
@@ -4201,9 +4118,8 @@
       <c r="L84" s="4"/>
       <c r="M84" s="4"/>
       <c r="N84" s="4"/>
-      <c r="O84" s="4"/>
-    </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="85" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A85" s="4" t="s">
         <v>150</v>
       </c>
@@ -4224,7 +4140,7 @@
       </c>
       <c r="G85" s="5"/>
       <c r="H85" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I85" s="4"/>
       <c r="J85" s="4"/>
@@ -4232,9 +4148,8 @@
       <c r="L85" s="4"/>
       <c r="M85" s="4"/>
       <c r="N85" s="4"/>
-      <c r="O85" s="4"/>
-    </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="86" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A86" s="4" t="s">
         <v>150</v>
       </c>
@@ -4255,7 +4170,7 @@
       </c>
       <c r="G86" s="6"/>
       <c r="H86" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I86" s="4"/>
       <c r="J86" s="4"/>
@@ -4263,9 +4178,8 @@
       <c r="L86" s="4"/>
       <c r="M86" s="4"/>
       <c r="N86" s="4"/>
-      <c r="O86" s="4"/>
-    </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="87" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A87" s="4" t="s">
         <v>150</v>
       </c>
@@ -4286,7 +4200,7 @@
       </c>
       <c r="G87" s="6"/>
       <c r="H87" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I87" s="4"/>
       <c r="J87" s="4"/>
@@ -4294,9 +4208,8 @@
       <c r="L87" s="4"/>
       <c r="M87" s="4"/>
       <c r="N87" s="4"/>
-      <c r="O87" s="4"/>
-    </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="88" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A88" s="4" t="s">
         <v>150</v>
       </c>
@@ -4317,7 +4230,7 @@
       </c>
       <c r="G88" s="6"/>
       <c r="H88" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I88" s="4"/>
       <c r="J88" s="4"/>
@@ -4325,9 +4238,8 @@
       <c r="L88" s="4"/>
       <c r="M88" s="4"/>
       <c r="N88" s="4"/>
-      <c r="O88" s="4"/>
-    </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="89" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A89" s="4" t="s">
         <v>150</v>
       </c>
@@ -4348,7 +4260,7 @@
       </c>
       <c r="G89" s="6"/>
       <c r="H89" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I89" s="4"/>
       <c r="J89" s="4"/>
@@ -4356,9 +4268,8 @@
       <c r="L89" s="4"/>
       <c r="M89" s="4"/>
       <c r="N89" s="4"/>
-      <c r="O89" s="4"/>
-    </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="90" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A90" s="4" t="s">
         <v>150</v>
       </c>
@@ -4381,7 +4292,7 @@
         <v>37</v>
       </c>
       <c r="H90" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I90" s="4"/>
       <c r="J90" s="4"/>
@@ -4389,9 +4300,8 @@
       <c r="L90" s="4"/>
       <c r="M90" s="4"/>
       <c r="N90" s="4"/>
-      <c r="O90" s="4"/>
-    </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="91" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A91" s="4" t="s">
         <v>150</v>
       </c>
@@ -4412,7 +4322,7 @@
       </c>
       <c r="G91" s="6"/>
       <c r="H91" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I91" s="4"/>
       <c r="J91" s="4"/>
@@ -4420,9 +4330,8 @@
       <c r="L91" s="4"/>
       <c r="M91" s="4"/>
       <c r="N91" s="4"/>
-      <c r="O91" s="4"/>
-    </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="92" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A92" s="4" t="s">
         <v>150</v>
       </c>
@@ -4443,7 +4352,7 @@
       </c>
       <c r="G92" s="6"/>
       <c r="H92" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I92" s="4"/>
       <c r="J92" s="4"/>
@@ -4451,9 +4360,8 @@
       <c r="L92" s="4"/>
       <c r="M92" s="4"/>
       <c r="N92" s="4"/>
-      <c r="O92" s="4"/>
-    </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="93" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A93" s="4" t="s">
         <v>150</v>
       </c>
@@ -4476,7 +4384,7 @@
         <v>37</v>
       </c>
       <c r="H93" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I93" s="4"/>
       <c r="J93" s="4"/>
@@ -4484,9 +4392,8 @@
       <c r="L93" s="4"/>
       <c r="M93" s="4"/>
       <c r="N93" s="4"/>
-      <c r="O93" s="4"/>
-    </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="94" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A94" s="4" t="s">
         <v>150</v>
       </c>
@@ -4507,7 +4414,7 @@
       </c>
       <c r="G94" s="6"/>
       <c r="H94" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I94" s="4"/>
       <c r="J94" s="4"/>
@@ -4515,9 +4422,8 @@
       <c r="L94" s="4"/>
       <c r="M94" s="4"/>
       <c r="N94" s="4"/>
-      <c r="O94" s="4"/>
-    </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="95" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A95" s="4" t="s">
         <v>150</v>
       </c>
@@ -4540,7 +4446,7 @@
         <v>255</v>
       </c>
       <c r="H95" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I95" s="4"/>
       <c r="J95" s="4"/>
@@ -4548,9 +4454,8 @@
       <c r="L95" s="4"/>
       <c r="M95" s="4"/>
       <c r="N95" s="4"/>
-      <c r="O95" s="4"/>
-    </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="96" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A96" s="4" t="s">
         <v>150</v>
       </c>
@@ -4573,7 +4478,7 @@
         <v>258</v>
       </c>
       <c r="H96" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I96" s="4"/>
       <c r="J96" s="4"/>
@@ -4581,9 +4486,8 @@
       <c r="L96" s="4"/>
       <c r="M96" s="4"/>
       <c r="N96" s="4"/>
-      <c r="O96" s="4"/>
-    </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="97" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A97" s="4" t="s">
         <v>150</v>
       </c>
@@ -4606,7 +4510,7 @@
         <v>277</v>
       </c>
       <c r="H97" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I97" s="4"/>
       <c r="J97" s="4"/>
@@ -4614,9 +4518,8 @@
       <c r="L97" s="4"/>
       <c r="M97" s="4"/>
       <c r="N97" s="4"/>
-      <c r="O97" s="4"/>
-    </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="98" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A98" s="4" t="s">
         <v>150</v>
       </c>
@@ -4624,7 +4527,7 @@
         <v>302</v>
       </c>
       <c r="C98" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D98" s="4" t="s">
         <v>159</v>
@@ -4639,7 +4542,7 @@
         <v>262</v>
       </c>
       <c r="H98" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I98" s="4"/>
       <c r="J98" s="4"/>
@@ -4647,9 +4550,8 @@
       <c r="L98" s="4"/>
       <c r="M98" s="4"/>
       <c r="N98" s="4"/>
-      <c r="O98" s="4"/>
-    </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="99" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A99" s="4" t="s">
         <v>150</v>
       </c>
@@ -4670,7 +4572,7 @@
       </c>
       <c r="G99" s="6"/>
       <c r="H99" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I99" s="4"/>
       <c r="J99" s="4"/>
@@ -4678,9 +4580,8 @@
       <c r="L99" s="4"/>
       <c r="M99" s="4"/>
       <c r="N99" s="4"/>
-      <c r="O99" s="4"/>
-    </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="100" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A100" s="4" t="s">
         <v>150</v>
       </c>
@@ -4688,13 +4589,13 @@
         <v>304</v>
       </c>
       <c r="C100" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D100" s="4" t="s">
         <v>159</v>
       </c>
       <c r="E100" s="4" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="F100" s="4" t="s">
         <v>36</v>
@@ -4703,7 +4604,7 @@
         <v>37</v>
       </c>
       <c r="H100" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I100" s="4"/>
       <c r="J100" s="4"/>
@@ -4711,9 +4612,8 @@
       <c r="L100" s="4"/>
       <c r="M100" s="4"/>
       <c r="N100" s="4"/>
-      <c r="O100" s="4"/>
-    </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="101" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A101" s="4" t="s">
         <v>150</v>
       </c>
@@ -4721,19 +4621,19 @@
         <v>305</v>
       </c>
       <c r="C101" s="4" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D101" s="4" t="s">
         <v>159</v>
       </c>
       <c r="E101" s="4" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="F101" s="4" t="s">
         <v>57</v>
       </c>
       <c r="G101" s="6" t="s">
-        <v>327</v>
+        <v>339</v>
       </c>
       <c r="H101" t="s">
         <v>340</v>
@@ -4744,9 +4644,8 @@
       <c r="L101" s="4"/>
       <c r="M101" s="4"/>
       <c r="N101" s="4"/>
-      <c r="O101" s="4"/>
-    </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="102" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A102" s="4" t="s">
         <v>150</v>
       </c>
@@ -4754,13 +4653,13 @@
         <v>306</v>
       </c>
       <c r="C102" s="4" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="D102" s="4" t="s">
         <v>159</v>
       </c>
       <c r="E102" s="4" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="F102" s="4" t="s">
         <v>57</v>
@@ -4768,16 +4667,17 @@
       <c r="G102" s="6" t="s">
         <v>239</v>
       </c>
-      <c r="H102" s="4"/>
+      <c r="H102" t="s">
+        <v>340</v>
+      </c>
       <c r="I102" s="4"/>
       <c r="J102" s="4"/>
       <c r="K102" s="4"/>
       <c r="L102" s="4"/>
       <c r="M102" s="4"/>
       <c r="N102" s="4"/>
-      <c r="O102" s="4"/>
-    </row>
-    <row r="103" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="103" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A103" s="4" t="s">
         <v>150</v>
       </c>
@@ -4785,30 +4685,31 @@
         <v>307</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="D103" s="4" t="s">
         <v>159</v>
       </c>
       <c r="E103" s="4" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="F103" s="4" t="s">
         <v>57</v>
       </c>
       <c r="G103" s="6" t="s">
-        <v>332</v>
-      </c>
-      <c r="H103" s="4"/>
+        <v>330</v>
+      </c>
+      <c r="H103" t="s">
+        <v>340</v>
+      </c>
       <c r="I103" s="4"/>
       <c r="J103" s="4"/>
       <c r="K103" s="4"/>
       <c r="L103" s="4"/>
       <c r="M103" s="4"/>
       <c r="N103" s="4"/>
-      <c r="O103" s="4"/>
-    </row>
-    <row r="104" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="104" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A104" s="4" t="s">
         <v>150</v>
       </c>
@@ -4828,16 +4729,17 @@
         <v>27</v>
       </c>
       <c r="G104" s="6"/>
-      <c r="H104" s="4"/>
+      <c r="H104" t="s">
+        <v>340</v>
+      </c>
       <c r="I104" s="4"/>
       <c r="J104" s="4"/>
       <c r="K104" s="4"/>
       <c r="L104" s="4"/>
       <c r="M104" s="4"/>
       <c r="N104" s="4"/>
-      <c r="O104" s="4"/>
-    </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="105" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A105" s="4" t="s">
         <v>150</v>
       </c>
@@ -4845,28 +4747,29 @@
         <v>309</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D105" s="4" t="s">
         <v>159</v>
       </c>
       <c r="E105" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="F105" s="4" t="s">
         <v>27</v>
       </c>
       <c r="G105" s="6"/>
-      <c r="H105" s="4"/>
+      <c r="H105" t="s">
+        <v>340</v>
+      </c>
       <c r="I105" s="4"/>
       <c r="J105" s="4"/>
       <c r="K105" s="4"/>
       <c r="L105" s="4"/>
       <c r="M105" s="4"/>
       <c r="N105" s="4"/>
-      <c r="O105" s="4"/>
-    </row>
-    <row r="106" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="106" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A106" s="4" t="s">
         <v>150</v>
       </c>
@@ -4886,16 +4789,17 @@
         <v>27</v>
       </c>
       <c r="G106" s="6"/>
-      <c r="H106" s="4"/>
+      <c r="H106" t="s">
+        <v>340</v>
+      </c>
       <c r="I106" s="4"/>
       <c r="J106" s="4"/>
       <c r="K106" s="4"/>
       <c r="L106" s="4"/>
       <c r="M106" s="4"/>
       <c r="N106" s="4"/>
-      <c r="O106" s="4"/>
-    </row>
-    <row r="107" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="107" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A107" s="4" t="s">
         <v>150</v>
       </c>
@@ -4911,16 +4815,17 @@
         <v>54</v>
       </c>
       <c r="G107" s="4"/>
-      <c r="H107" s="4"/>
+      <c r="H107" t="s">
+        <v>340</v>
+      </c>
       <c r="I107" s="4"/>
       <c r="J107" s="4"/>
       <c r="K107" s="4"/>
       <c r="L107" s="4"/>
       <c r="M107" s="4"/>
       <c r="N107" s="4"/>
-      <c r="O107" s="4"/>
-    </row>
-    <row r="108" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="108" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A108" s="4" t="s">
         <v>151</v>
       </c>
@@ -4945,9 +4850,8 @@
       <c r="L108" s="4"/>
       <c r="M108" s="4"/>
       <c r="N108" s="4"/>
-      <c r="O108" s="4"/>
-    </row>
-    <row r="109" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="109" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A109" s="4" t="s">
         <v>151</v>
       </c>
@@ -4970,9 +4874,8 @@
       <c r="L109" s="4"/>
       <c r="M109" s="4"/>
       <c r="N109" s="4"/>
-      <c r="O109" s="4"/>
-    </row>
-    <row r="110" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="110" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A110" s="4" t="s">
         <v>151</v>
       </c>
@@ -5001,9 +4904,8 @@
       <c r="L110" s="4"/>
       <c r="M110" s="4"/>
       <c r="N110" s="4"/>
-      <c r="O110" s="4"/>
-    </row>
-    <row r="111" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="111" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A111" s="4" t="s">
         <v>151</v>
       </c>
@@ -5032,9 +4934,8 @@
       <c r="L111" s="4"/>
       <c r="M111" s="4"/>
       <c r="N111" s="4"/>
-      <c r="O111" s="4"/>
-    </row>
-    <row r="112" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="112" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A112" s="4" t="s">
         <v>151</v>
       </c>
@@ -5063,9 +4964,8 @@
       <c r="L112" s="4"/>
       <c r="M112" s="4"/>
       <c r="N112" s="4"/>
-      <c r="O112" s="4"/>
-    </row>
-    <row r="113" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="113" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A113" s="4" t="s">
         <v>151</v>
       </c>
@@ -5092,9 +4992,8 @@
       <c r="L113" s="4"/>
       <c r="M113" s="4"/>
       <c r="N113" s="4"/>
-      <c r="O113" s="4"/>
-    </row>
-    <row r="114" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="114" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A114" s="4" t="s">
         <v>151</v>
       </c>
@@ -5121,9 +5020,8 @@
       <c r="L114" s="4"/>
       <c r="M114" s="4"/>
       <c r="N114" s="4"/>
-      <c r="O114" s="4"/>
-    </row>
-    <row r="115" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="115" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A115" s="4" t="s">
         <v>151</v>
       </c>
@@ -5152,14 +5050,13 @@
       <c r="L115" s="4"/>
       <c r="M115" s="4"/>
       <c r="N115" s="4"/>
-      <c r="O115" s="4"/>
-    </row>
-    <row r="116" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="116" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A116" s="4" t="s">
         <v>151</v>
       </c>
       <c r="B116" s="4" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C116" s="4" t="s">
         <v>28</v>
@@ -5181,14 +5078,13 @@
       <c r="L116" s="4"/>
       <c r="M116" s="4"/>
       <c r="N116" s="4"/>
-      <c r="O116" s="4"/>
-    </row>
-    <row r="117" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="117" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A117" s="4" t="s">
         <v>151</v>
       </c>
       <c r="B117" s="4" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C117" s="4" t="s">
         <v>32</v>
@@ -5210,14 +5106,13 @@
       <c r="L117" s="4"/>
       <c r="M117" s="4"/>
       <c r="N117" s="4"/>
-      <c r="O117" s="4"/>
-    </row>
-    <row r="118" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="118" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A118" s="4" t="s">
         <v>151</v>
       </c>
       <c r="B118" s="4" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C118" s="4" t="s">
         <v>60</v>
@@ -5241,14 +5136,13 @@
       <c r="L118" s="4"/>
       <c r="M118" s="4"/>
       <c r="N118" s="4"/>
-      <c r="O118" s="4"/>
-    </row>
-    <row r="119" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="119" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A119" s="4" t="s">
         <v>151</v>
       </c>
       <c r="B119" s="4" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="C119" s="4" t="s">
         <v>61</v>
@@ -5270,14 +5164,13 @@
       <c r="L119" s="4"/>
       <c r="M119" s="4"/>
       <c r="N119" s="4"/>
-      <c r="O119" s="4"/>
-    </row>
-    <row r="120" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="120" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A120" s="4" t="s">
         <v>151</v>
       </c>
       <c r="B120" s="4" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C120" s="4" t="s">
         <v>62</v>
@@ -5299,14 +5192,13 @@
       <c r="L120" s="4"/>
       <c r="M120" s="4"/>
       <c r="N120" s="4"/>
-      <c r="O120" s="4"/>
-    </row>
-    <row r="121" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="121" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A121" s="4" t="s">
         <v>151</v>
       </c>
       <c r="B121" s="4" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C121" s="4" t="s">
         <v>63</v>
@@ -5330,14 +5222,13 @@
       <c r="L121" s="4"/>
       <c r="M121" s="4"/>
       <c r="N121" s="4"/>
-      <c r="O121" s="4"/>
-    </row>
-    <row r="122" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="122" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A122" s="4" t="s">
         <v>151</v>
       </c>
       <c r="B122" s="4" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C122" s="4" t="s">
         <v>64</v>
@@ -5355,9 +5246,8 @@
       <c r="L122" s="4"/>
       <c r="M122" s="4"/>
       <c r="N122" s="4"/>
-      <c r="O122" s="4"/>
-    </row>
-    <row r="123" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="123" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A123" s="4"/>
       <c r="B123" s="4"/>
       <c r="C123" s="4"/>
@@ -5372,9 +5262,8 @@
       <c r="L123" s="4"/>
       <c r="M123" s="4"/>
       <c r="N123" s="4"/>
-      <c r="O123" s="4"/>
-    </row>
-    <row r="124" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="124" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A124" s="4"/>
       <c r="B124" s="4"/>
       <c r="C124" s="4"/>
@@ -5389,9 +5278,8 @@
       <c r="L124" s="4"/>
       <c r="M124" s="4"/>
       <c r="N124" s="4"/>
-      <c r="O124" s="4"/>
-    </row>
-    <row r="125" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="125" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A125" s="4"/>
       <c r="B125" s="4"/>
       <c r="C125" s="4"/>
@@ -5406,9 +5294,8 @@
       <c r="L125" s="4"/>
       <c r="M125" s="4"/>
       <c r="N125" s="4"/>
-      <c r="O125" s="4"/>
-    </row>
-    <row r="126" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="126" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A126" s="4"/>
       <c r="B126" s="4"/>
       <c r="C126" s="4"/>
@@ -5423,9 +5310,8 @@
       <c r="L126" s="4"/>
       <c r="M126" s="4"/>
       <c r="N126" s="4"/>
-      <c r="O126" s="4"/>
-    </row>
-    <row r="127" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="127" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A127" s="4"/>
       <c r="B127" s="4"/>
       <c r="C127" s="4"/>
@@ -5440,9 +5326,8 @@
       <c r="L127" s="4"/>
       <c r="M127" s="4"/>
       <c r="N127" s="4"/>
-      <c r="O127" s="4"/>
-    </row>
-    <row r="128" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="128" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A128" s="4"/>
       <c r="B128" s="4"/>
       <c r="C128" s="4"/>
@@ -5457,9 +5342,8 @@
       <c r="L128" s="4"/>
       <c r="M128" s="4"/>
       <c r="N128" s="4"/>
-      <c r="O128" s="4"/>
-    </row>
-    <row r="129" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="129" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A129" s="4"/>
       <c r="B129" s="4"/>
       <c r="C129" s="4"/>
@@ -5474,9 +5358,8 @@
       <c r="L129" s="4"/>
       <c r="M129" s="4"/>
       <c r="N129" s="4"/>
-      <c r="O129" s="4"/>
-    </row>
-    <row r="130" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="130" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A130" s="4"/>
       <c r="B130" s="4"/>
       <c r="C130" s="4"/>
@@ -5491,9 +5374,8 @@
       <c r="L130" s="4"/>
       <c r="M130" s="4"/>
       <c r="N130" s="4"/>
-      <c r="O130" s="4"/>
-    </row>
-    <row r="131" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="131" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A131" s="4"/>
       <c r="B131" s="4"/>
       <c r="C131" s="4"/>
@@ -5508,9 +5390,8 @@
       <c r="L131" s="4"/>
       <c r="M131" s="4"/>
       <c r="N131" s="4"/>
-      <c r="O131" s="4"/>
-    </row>
-    <row r="132" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="132" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A132" s="4"/>
       <c r="B132" s="4"/>
       <c r="C132" s="4"/>
@@ -5525,9 +5406,8 @@
       <c r="L132" s="4"/>
       <c r="M132" s="4"/>
       <c r="N132" s="4"/>
-      <c r="O132" s="4"/>
-    </row>
-    <row r="133" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="133" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A133" s="4"/>
       <c r="B133" s="4"/>
       <c r="C133" s="4"/>
@@ -5542,9 +5422,8 @@
       <c r="L133" s="4"/>
       <c r="M133" s="4"/>
       <c r="N133" s="4"/>
-      <c r="O133" s="4"/>
-    </row>
-    <row r="134" spans="1:15" x14ac:dyDescent="0.45">
+    </row>
+    <row r="134" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A134" s="4"/>
       <c r="B134" s="4"/>
       <c r="C134" s="4"/>
@@ -5559,160 +5438,6 @@
       <c r="L134" s="4"/>
       <c r="M134" s="4"/>
       <c r="N134" s="4"/>
-      <c r="O134" s="4"/>
-    </row>
-    <row r="135" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A135" s="4"/>
-      <c r="B135" s="4"/>
-      <c r="C135" s="4"/>
-      <c r="D135" s="4"/>
-      <c r="E135" s="4"/>
-      <c r="F135" s="4"/>
-      <c r="G135" s="4"/>
-      <c r="H135" s="4"/>
-      <c r="I135" s="4"/>
-      <c r="J135" s="4"/>
-      <c r="K135" s="4"/>
-      <c r="L135" s="4"/>
-      <c r="M135" s="4"/>
-      <c r="N135" s="4"/>
-      <c r="O135" s="4"/>
-    </row>
-    <row r="136" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A136" s="4"/>
-      <c r="B136" s="4"/>
-      <c r="C136" s="4"/>
-      <c r="D136" s="4"/>
-      <c r="E136" s="4"/>
-      <c r="F136" s="4"/>
-      <c r="G136" s="4"/>
-      <c r="H136" s="4"/>
-      <c r="I136" s="4"/>
-      <c r="J136" s="4"/>
-      <c r="K136" s="4"/>
-      <c r="L136" s="4"/>
-      <c r="M136" s="4"/>
-      <c r="N136" s="4"/>
-      <c r="O136" s="4"/>
-    </row>
-    <row r="137" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A137" s="4"/>
-      <c r="B137" s="4"/>
-      <c r="C137" s="4"/>
-      <c r="D137" s="4"/>
-      <c r="E137" s="4"/>
-      <c r="F137" s="4"/>
-      <c r="G137" s="4"/>
-      <c r="H137" s="4"/>
-      <c r="I137" s="4"/>
-      <c r="J137" s="4"/>
-      <c r="K137" s="4"/>
-      <c r="L137" s="4"/>
-      <c r="M137" s="4"/>
-      <c r="N137" s="4"/>
-      <c r="O137" s="4"/>
-    </row>
-    <row r="138" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A138" s="4"/>
-      <c r="B138" s="4"/>
-      <c r="C138" s="4"/>
-      <c r="D138" s="4"/>
-      <c r="E138" s="4"/>
-      <c r="F138" s="4"/>
-      <c r="G138" s="4"/>
-      <c r="H138" s="4"/>
-      <c r="I138" s="4"/>
-      <c r="J138" s="4"/>
-      <c r="K138" s="4"/>
-      <c r="L138" s="4"/>
-      <c r="M138" s="4"/>
-      <c r="N138" s="4"/>
-      <c r="O138" s="4"/>
-    </row>
-    <row r="139" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A139" s="4"/>
-      <c r="B139" s="4"/>
-      <c r="C139" s="4"/>
-      <c r="D139" s="4"/>
-      <c r="E139" s="4"/>
-      <c r="F139" s="4"/>
-      <c r="G139" s="4"/>
-      <c r="H139" s="4"/>
-      <c r="I139" s="4"/>
-      <c r="J139" s="4"/>
-      <c r="K139" s="4"/>
-      <c r="L139" s="4"/>
-      <c r="M139" s="4"/>
-      <c r="N139" s="4"/>
-      <c r="O139" s="4"/>
-    </row>
-    <row r="140" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A140" s="4"/>
-      <c r="B140" s="4"/>
-      <c r="C140" s="4"/>
-      <c r="D140" s="4"/>
-      <c r="E140" s="4"/>
-      <c r="F140" s="4"/>
-      <c r="G140" s="4"/>
-      <c r="H140" s="4"/>
-      <c r="I140" s="4"/>
-      <c r="J140" s="4"/>
-      <c r="K140" s="4"/>
-      <c r="L140" s="4"/>
-      <c r="M140" s="4"/>
-      <c r="N140" s="4"/>
-      <c r="O140" s="4"/>
-    </row>
-    <row r="141" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A141" s="4"/>
-      <c r="B141" s="4"/>
-      <c r="C141" s="4"/>
-      <c r="D141" s="4"/>
-      <c r="E141" s="4"/>
-      <c r="F141" s="4"/>
-      <c r="G141" s="4"/>
-      <c r="H141" s="4"/>
-      <c r="I141" s="4"/>
-      <c r="J141" s="4"/>
-      <c r="K141" s="4"/>
-      <c r="L141" s="4"/>
-      <c r="M141" s="4"/>
-      <c r="N141" s="4"/>
-      <c r="O141" s="4"/>
-    </row>
-    <row r="142" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A142" s="4"/>
-      <c r="B142" s="4"/>
-      <c r="C142" s="4"/>
-      <c r="D142" s="4"/>
-      <c r="E142" s="4"/>
-      <c r="F142" s="4"/>
-      <c r="G142" s="4"/>
-      <c r="H142" s="4"/>
-      <c r="I142" s="4"/>
-      <c r="J142" s="4"/>
-      <c r="K142" s="4"/>
-      <c r="L142" s="4"/>
-      <c r="M142" s="4"/>
-      <c r="N142" s="4"/>
-      <c r="O142" s="4"/>
-    </row>
-    <row r="143" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A143" s="4"/>
-      <c r="B143" s="4"/>
-      <c r="C143" s="4"/>
-      <c r="D143" s="4"/>
-      <c r="E143" s="4"/>
-      <c r="F143" s="4"/>
-      <c r="G143" s="4"/>
-      <c r="H143" s="4"/>
-      <c r="I143" s="4"/>
-      <c r="J143" s="4"/>
-      <c r="K143" s="4"/>
-      <c r="L143" s="4"/>
-      <c r="M143" s="4"/>
-      <c r="N143" s="4"/>
-      <c r="O143" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>